<commit_message>
updated data Feb 8
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="72">
   <si>
     <t>Male</t>
   </si>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -728,7 +728,9 @@
         <v>6</v>
       </c>
       <c r="J3" s="7"/>
-      <c r="K3" s="5"/>
+      <c r="K3" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="5">

</xml_diff>

<commit_message>
updated on Feb 08 night
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="89">
   <si>
     <t>Male</t>
   </si>
@@ -258,6 +258,57 @@
   </si>
   <si>
     <t>Victoria Junior College, Parkway East Hospital, Changi Airport, Singapore Zoo</t>
+  </si>
+  <si>
+    <t>Sin Ming Road</t>
+  </si>
+  <si>
+    <t>Yong Thai Hang, GP Clinic, NCID</t>
+  </si>
+  <si>
+    <t>Henderson Crescent</t>
+  </si>
+  <si>
+    <t>Bukit Merah Polyclinic, SGH, Redhill Market, Hawker centre at Bukit Merah</t>
+  </si>
+  <si>
+    <t>Bukit Batok Street 31</t>
+  </si>
+  <si>
+    <t>Jurong East Street 32</t>
+  </si>
+  <si>
+    <t>GP clinics, Ng Teng Fong General Hospital, NCID</t>
+  </si>
+  <si>
+    <t>Feb-08</t>
+  </si>
+  <si>
+    <t>Choa Chu Kang Polyclinic, The Life Church and Missions Singapore, Marina Bay Sands, Chinatown and Plaza Singapura</t>
+  </si>
+  <si>
+    <t>Choa Chu Kang Avenue 3</t>
+  </si>
+  <si>
+    <t>Malaysia, GP clinics, NCID, Grand Hyatt Singapore</t>
+  </si>
+  <si>
+    <t>Jurong West Central</t>
+  </si>
+  <si>
+    <t>GP clinic, Yong Thai Hang</t>
+  </si>
+  <si>
+    <t>Bedok North Street</t>
+  </si>
+  <si>
+    <t>Grand Hyatt Singapore, Johor Bahru, GP clinic, NCID, KK Women’s and Children’s Hospital, Ng Teng Fong General Hospital</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -614,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1709,6 +1760,237 @@
       <c r="J34" s="7"/>
       <c r="K34" s="5"/>
     </row>
+    <row r="35" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5">
+        <v>1.355904</v>
+      </c>
+      <c r="C35" s="5">
+        <v>103.838301</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" s="5">
+        <v>40</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="K35" s="5"/>
+    </row>
+    <row r="36" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5">
+        <v>1.2887710000000001</v>
+      </c>
+      <c r="C36" s="5">
+        <v>103.821619</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" s="5">
+        <v>64</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J36" s="7"/>
+      <c r="K36" s="5"/>
+    </row>
+    <row r="37" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="5">
+        <v>1.359237</v>
+      </c>
+      <c r="C37" s="5">
+        <v>103.75111699999999</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" s="5">
+        <v>38</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K37" s="5"/>
+    </row>
+    <row r="38" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="5">
+        <v>1.3472470000000001</v>
+      </c>
+      <c r="C38" s="5">
+        <v>103.73366300000001</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" s="5">
+        <v>53</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J38" s="7"/>
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5">
+        <v>1.380107</v>
+      </c>
+      <c r="C39" s="5">
+        <v>103.741224</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" s="5">
+        <v>52</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J39" s="7"/>
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="5">
+        <v>1.3424970000000001</v>
+      </c>
+      <c r="C40" s="5">
+        <v>103.705433</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" s="5">
+        <v>51</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J40" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" s="5">
+        <v>1.3330010000000001</v>
+      </c>
+      <c r="C41" s="5">
+        <v>103.926856</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" s="5">
+        <v>36</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="K41" s="5"/>
+    </row>
+    <row r="42" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+    </row>
+    <row r="43" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update on Feb 9
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="94">
   <si>
     <t>Male</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Singapore</t>
   </si>
   <si>
-    <t>Arrived in Singapore</t>
-  </si>
-  <si>
     <t>Nathan Road</t>
   </si>
   <si>
@@ -236,9 +233,6 @@
     <t>Grand Hyatt Singapore Hotel</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
     <t>Feb-07</t>
   </si>
   <si>
@@ -309,6 +303,27 @@
   </si>
   <si>
     <t>30</t>
+  </si>
+  <si>
+    <t>Arrived from Wuhan</t>
+  </si>
+  <si>
+    <t>GP Clinic, Hougang Polyclinic, Tan Tock Seng Hospital’s emergency department, Paya Lebar Methodist Church, Braddell Heights Residents, Pat’s Schoolhouse Kovan</t>
+  </si>
+  <si>
+    <t>755 Upper Serangoon Road</t>
+  </si>
+  <si>
+    <t>Changi General Hospital, Bedok Polyclinic, Mustafa Centre</t>
+  </si>
+  <si>
+    <t>The Leo dormitory (25 Kaki Bukit Road)</t>
+  </si>
+  <si>
+    <t>Malaysia, Sengkang General Hospital, Resorts World Sentosa</t>
+  </si>
+  <si>
+    <t>Fernvale Close</t>
   </si>
 </sst>
 </file>
@@ -665,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -679,44 +694,44 @@
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.33203125" customWidth="1"/>
+    <col min="8" max="8" width="54.6640625" customWidth="1"/>
     <col min="9" max="9" width="42.83203125" customWidth="1"/>
     <col min="10" max="10" width="23.6640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.25">
@@ -730,7 +745,7 @@
         <v>103.80979619999999</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" s="5">
         <v>66</v>
@@ -761,7 +776,7 @@
         <v>103.8585204</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" s="5">
         <v>53</v>
@@ -780,7 +795,7 @@
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
@@ -794,7 +809,7 @@
         <v>103.810018</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="5">
         <v>37</v>
@@ -827,7 +842,7 @@
         <v>103.820006847</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="5">
         <v>36</v>
@@ -858,7 +873,7 @@
         <v>103.900929093</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" s="5">
         <v>56</v>
@@ -889,7 +904,7 @@
         <v>103.944834173</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" s="5">
         <v>56</v>
@@ -908,7 +923,7 @@
       </c>
       <c r="J7" s="7"/>
       <c r="K7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.25">
@@ -922,7 +937,7 @@
         <v>103.860577941</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="5">
         <v>35</v>
@@ -953,7 +968,7 @@
         <v>103.87764483700001</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="5">
         <v>56</v>
@@ -984,7 +999,7 @@
         <v>103.87756705300001</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="5">
         <v>56</v>
@@ -1015,7 +1030,7 @@
         <v>103.8631688</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="5">
         <v>56</v>
@@ -1048,7 +1063,7 @@
         <v>103.820199966</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="5">
         <v>31</v>
@@ -1079,7 +1094,7 @@
         <v>103.819829822</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="5">
         <v>37</v>
@@ -1110,7 +1125,7 @@
         <v>103.846496344</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E14" s="5">
         <v>73</v>
@@ -1141,7 +1156,7 @@
         <v>103.737467229</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15" s="5">
         <v>31</v>
@@ -1172,7 +1187,7 @@
         <v>103.99087428999999</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="5">
         <v>47</v>
@@ -1184,7 +1199,7 @@
         <v>25</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>1</v>
@@ -1203,7 +1218,7 @@
         <v>103.8256719</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" s="5">
         <v>38</v>
@@ -1215,7 +1230,7 @@
         <v>22</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>3</v>
@@ -1234,7 +1249,7 @@
         <v>103.991131783</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" s="5">
         <v>47</v>
@@ -1246,7 +1261,7 @@
         <v>25</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>1</v>
@@ -1267,7 +1282,7 @@
         <v>103.878130317</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="5">
         <v>31</v>
@@ -1279,10 +1294,10 @@
         <v>1</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="5"/>
@@ -1298,7 +1313,7 @@
         <v>103.81527811300001</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" s="5">
         <v>28</v>
@@ -1310,10 +1325,10 @@
         <v>25</v>
       </c>
       <c r="H20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="J20" s="7"/>
       <c r="K20" s="5"/>
@@ -1329,7 +1344,7 @@
         <v>103.885970414</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E21" s="5">
         <v>48</v>
@@ -1341,10 +1356,10 @@
         <v>25</v>
       </c>
       <c r="H21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="J21" s="7">
         <v>19</v>
@@ -1362,7 +1377,7 @@
         <v>103.815087676</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" s="5">
         <v>44</v>
@@ -1374,10 +1389,10 @@
         <v>25</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J22" s="7">
         <v>19</v>
@@ -1395,7 +1410,7 @@
         <v>103.99122566</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" s="5">
         <v>41</v>
@@ -1407,7 +1422,7 @@
         <v>25</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>1</v>
@@ -1426,7 +1441,7 @@
         <v>103.99096548599999</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="5">
         <v>17</v>
@@ -1438,7 +1453,7 @@
         <v>25</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>1</v>
@@ -1457,7 +1472,7 @@
         <v>103.8826748</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E25" s="5">
         <v>32</v>
@@ -1469,10 +1484,10 @@
         <v>25</v>
       </c>
       <c r="H25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="J25" s="7">
         <v>19</v>
@@ -1490,7 +1505,7 @@
         <v>103.882692754</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" s="5">
         <v>32</v>
@@ -1502,10 +1517,10 @@
         <v>25</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J26" s="7">
         <v>24</v>
@@ -1523,7 +1538,7 @@
         <v>103.847638965</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" s="5">
         <v>42</v>
@@ -1534,9 +1549,11 @@
       <c r="G27" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="5"/>
+      <c r="H27" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="I27" s="5" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="J27" s="7">
         <v>13</v>
@@ -1554,7 +1571,7 @@
         <v>103.81559461400001</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E28" s="5">
         <v>45</v>
@@ -1566,10 +1583,10 @@
         <v>25</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J28" s="7">
         <v>19</v>
@@ -1587,7 +1604,7 @@
         <v>103.815433681</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E29" s="5">
         <v>0.6</v>
@@ -1599,10 +1616,10 @@
         <v>25</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J29" s="7">
         <v>27</v>
@@ -1620,7 +1637,7 @@
         <v>103.84413499999999</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E30" s="5">
         <v>41</v>
@@ -1633,7 +1650,7 @@
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J30" s="7"/>
       <c r="K30" s="5"/>
@@ -1649,7 +1666,7 @@
         <v>103.833184</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E31" s="5">
         <v>27</v>
@@ -1662,7 +1679,7 @@
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J31" s="7"/>
       <c r="K31" s="5"/>
@@ -1678,7 +1695,7 @@
         <v>103.95156299999999</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E32" s="5">
         <v>53</v>
@@ -1690,10 +1707,10 @@
         <v>25</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J32" s="7"/>
       <c r="K32" s="5"/>
@@ -1709,7 +1726,7 @@
         <v>103.94172</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E33" s="5">
         <v>42</v>
@@ -1721,10 +1738,10 @@
         <v>25</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J33" s="7"/>
       <c r="K33" s="5"/>
@@ -1740,7 +1757,7 @@
         <v>103.894414</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E34" s="5">
         <v>39</v>
@@ -1752,10 +1769,10 @@
         <v>25</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J34" s="7"/>
       <c r="K34" s="5"/>
@@ -1771,7 +1788,7 @@
         <v>103.838301</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E35" s="5">
         <v>40</v>
@@ -1783,13 +1800,13 @@
         <v>25</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J35" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K35" s="5"/>
     </row>
@@ -1804,7 +1821,7 @@
         <v>103.821619</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E36" s="5">
         <v>64</v>
@@ -1816,10 +1833,10 @@
         <v>25</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J36" s="7"/>
       <c r="K36" s="5"/>
@@ -1835,7 +1852,7 @@
         <v>103.75111699999999</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E37" s="5">
         <v>38</v>
@@ -1847,13 +1864,13 @@
         <v>25</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I37" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J37" s="7" t="s">
         <v>86</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="K37" s="5"/>
     </row>
@@ -1868,7 +1885,7 @@
         <v>103.73366300000001</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E38" s="5">
         <v>53</v>
@@ -1880,10 +1897,10 @@
         <v>25</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J38" s="7"/>
       <c r="K38" s="5"/>
@@ -1899,7 +1916,7 @@
         <v>103.741224</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E39" s="5">
         <v>52</v>
@@ -1911,10 +1928,10 @@
         <v>25</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J39" s="7"/>
       <c r="K39" s="5"/>
@@ -1930,7 +1947,7 @@
         <v>103.705433</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E40" s="5">
         <v>51</v>
@@ -1942,13 +1959,13 @@
         <v>25</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K40" s="5"/>
     </row>
@@ -1963,7 +1980,7 @@
         <v>103.926856</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E41" s="5">
         <v>36</v>
@@ -1975,21 +1992,108 @@
         <v>25</v>
       </c>
       <c r="H41" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J41" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="K41" s="5"/>
     </row>
     <row r="42" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" s="5">
+        <v>1.3543160000000001</v>
+      </c>
+      <c r="C42" s="5">
+        <v>103.878049</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="5">
+        <v>71</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J42" s="7"/>
+      <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
+      <c r="A43" s="5">
+        <v>42</v>
+      </c>
+      <c r="B43" s="5">
+        <v>1.3397490000000001</v>
+      </c>
+      <c r="C43" s="5">
+        <v>103.910634</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" s="5">
+        <v>39</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="J43" s="7"/>
+      <c r="K43" s="5"/>
+    </row>
+    <row r="44" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" s="5">
+        <v>1.3944110000000001</v>
+      </c>
+      <c r="C44" s="5">
+        <v>103.880578</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="5">
+        <v>54</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J44" s="7"/>
+      <c r="K44" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update on Feb 10
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="99">
   <si>
     <t>Male</t>
   </si>
@@ -324,6 +324,21 @@
   </si>
   <si>
     <t>Fernvale Close</t>
+  </si>
+  <si>
+    <t>Feb-09</t>
+  </si>
+  <si>
+    <t>Certis Cisco Centre (20 Jalan Afifi), Chingay 2020, Khoo Teck Puat Hospital (KTPH)</t>
+  </si>
+  <si>
+    <t>Sembawang Drive</t>
+  </si>
+  <si>
+    <t>KK Women’s and Children’s Hospital</t>
+  </si>
+  <si>
+    <t>Feb-10</t>
   </si>
 </sst>
 </file>
@@ -680,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2095,6 +2110,68 @@
       <c r="J44" s="7"/>
       <c r="K44" s="5"/>
     </row>
+    <row r="45" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" s="5">
+        <v>1.452561</v>
+      </c>
+      <c r="C45" s="5">
+        <v>103.816625</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E45" s="5">
+        <v>37</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="J45" s="7"/>
+      <c r="K45" s="5"/>
+    </row>
+    <row r="46" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5">
+        <v>1.3105450000000001</v>
+      </c>
+      <c r="C46" s="5">
+        <v>103.84683800000001</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E46" s="5">
+        <v>2</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="J46" s="7"/>
+      <c r="K46" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update on Feb 11
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="113">
   <si>
     <t>Male</t>
   </si>
@@ -354,6 +354,33 @@
   </si>
   <si>
     <t>Feb-03</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Chinese (PR)</t>
+  </si>
+  <si>
+    <t>Indonesian</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>Johor Bahru</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>10 Seletar Aerospace Heights</t>
+  </si>
+  <si>
+    <t>Veerasamy Road</t>
+  </si>
+  <si>
+    <t>Johor Bahru, Resorts World Sentosa Casino, TTSH, NCID</t>
   </si>
 </sst>
 </file>
@@ -711,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,7 +752,7 @@
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5" customWidth="1"/>
+    <col min="8" max="8" width="55.1640625" customWidth="1"/>
     <col min="9" max="9" width="38.33203125" customWidth="1"/>
     <col min="10" max="10" width="23.6640625" style="5" customWidth="1"/>
     <col min="11" max="11" width="15.5" customWidth="1"/>
@@ -809,9 +836,12 @@
       <c r="J2" s="4"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M2" s="8">
+        <v>44562</v>
+      </c>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -886,9 +916,11 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M4" s="8">
+        <v>44562</v>
+      </c>
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -922,9 +954,11 @@
       <c r="J5" s="4"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M5" s="8">
+        <v>44562</v>
+      </c>
       <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -958,9 +992,11 @@
       <c r="J6" s="4"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M6" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M6" s="8">
+        <v>45292</v>
+      </c>
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -994,9 +1030,11 @@
       <c r="J7" s="4"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M7" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M7" s="8">
+        <v>45658</v>
+      </c>
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1070,9 +1108,11 @@
       <c r="J9" s="4"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M9" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M9" s="8">
+        <v>43466</v>
+      </c>
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1106,9 +1146,11 @@
       <c r="J10" s="4"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M10" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M10" s="8">
+        <v>43466</v>
+      </c>
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1224,9 +1266,11 @@
       <c r="J13" s="4"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M13" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M13" s="8">
+        <v>46023</v>
+      </c>
       <c r="N13" s="3"/>
     </row>
     <row r="14" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1300,9 +1344,11 @@
       <c r="J15" s="4"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M15" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M15" s="8">
+        <v>46753</v>
+      </c>
       <c r="N15" s="3"/>
     </row>
     <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1338,7 +1384,9 @@
       <c r="L16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M16" s="3"/>
+      <c r="M16" s="8">
+        <v>10959</v>
+      </c>
       <c r="N16" s="3"/>
     </row>
     <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1372,9 +1420,11 @@
       <c r="J17" s="4"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M17" s="8">
+        <v>44562</v>
+      </c>
       <c r="N17" s="3"/>
     </row>
     <row r="18" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1412,7 +1462,9 @@
       <c r="L18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M18" s="3"/>
+      <c r="M18" s="8">
+        <v>10959</v>
+      </c>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1446,9 +1498,11 @@
       <c r="J19" s="4"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M19" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M19" s="8">
+        <v>36923</v>
+      </c>
       <c r="N19" s="3"/>
     </row>
     <row r="20" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1482,9 +1536,11 @@
       <c r="J20" s="4"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M20" s="3"/>
+        <v>105</v>
+      </c>
+      <c r="M20" s="8">
+        <v>47119</v>
+      </c>
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1522,7 +1578,9 @@
       <c r="L21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M21" s="3"/>
+      <c r="M21" s="8">
+        <v>45658</v>
+      </c>
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1558,7 +1616,7 @@
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
@@ -1636,7 +1694,9 @@
       <c r="L24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M24" s="3"/>
+      <c r="M24" s="8">
+        <v>10959</v>
+      </c>
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1674,7 +1734,9 @@
       <c r="L25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M25" s="3"/>
+      <c r="M25" s="8">
+        <v>10959</v>
+      </c>
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1712,7 +1774,9 @@
       <c r="L26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M26" s="3"/>
+      <c r="M26" s="8">
+        <v>45292</v>
+      </c>
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1864,7 +1928,9 @@
       <c r="L30" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M30" s="3"/>
+      <c r="M30" s="8">
+        <v>46753</v>
+      </c>
       <c r="N30" s="3"/>
     </row>
     <row r="31" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1898,7 +1964,9 @@
       <c r="L31" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M31" s="3"/>
+      <c r="M31" s="8">
+        <v>43831</v>
+      </c>
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -1934,7 +2002,9 @@
       <c r="L32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M32" s="3"/>
+      <c r="M32" s="8">
+        <v>44927</v>
+      </c>
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -2006,7 +2076,9 @@
       <c r="L34" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M34" s="3"/>
+      <c r="M34" s="8">
+        <v>10959</v>
+      </c>
       <c r="N34" s="3"/>
     </row>
     <row r="35" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -2044,7 +2116,9 @@
       <c r="L35" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M35" s="3"/>
+      <c r="M35" s="8">
+        <v>46388</v>
+      </c>
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -2080,7 +2154,9 @@
       <c r="L36" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M36" s="3"/>
+      <c r="M36" s="8">
+        <v>11324</v>
+      </c>
       <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -2116,9 +2192,11 @@
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M37" s="3"/>
+        <v>105</v>
+      </c>
+      <c r="M37" s="8">
+        <v>45292</v>
+      </c>
       <c r="N37" s="3"/>
     </row>
     <row r="38" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -2154,7 +2232,9 @@
       <c r="L38" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M38" s="3"/>
+      <c r="M38" s="8">
+        <v>10959</v>
+      </c>
       <c r="N38" s="3"/>
     </row>
     <row r="39" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -2228,7 +2308,9 @@
       <c r="L40" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M40" s="3"/>
+      <c r="M40" s="8">
+        <v>47119</v>
+      </c>
       <c r="N40" s="3"/>
     </row>
     <row r="41" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -2266,7 +2348,9 @@
       <c r="L41" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M41" s="3"/>
+      <c r="M41" s="8">
+        <v>10959</v>
+      </c>
       <c r="N41" s="3"/>
     </row>
     <row r="42" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -2302,7 +2386,9 @@
       <c r="L42" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M42" s="3"/>
+      <c r="M42" s="8">
+        <v>36923</v>
+      </c>
       <c r="N42" s="3"/>
     </row>
     <row r="43" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -2336,7 +2422,7 @@
       <c r="J43" s="4"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
@@ -2374,7 +2460,9 @@
       <c r="L44" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M44" s="3"/>
+      <c r="M44" s="8">
+        <v>10959</v>
+      </c>
       <c r="N44" s="3"/>
     </row>
     <row r="45" spans="1:14" ht="21" x14ac:dyDescent="0.25">
@@ -2446,8 +2534,88 @@
       <c r="L46" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M46" s="3"/>
+      <c r="M46" s="8">
+        <v>10959</v>
+      </c>
       <c r="N46" s="3"/>
+    </row>
+    <row r="47" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3">
+        <v>1.2559439999999999</v>
+      </c>
+      <c r="C47" s="3">
+        <v>103.82021400000001</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E47" s="3">
+        <v>35</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J47" s="4"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M47" s="8">
+        <v>38384</v>
+      </c>
+      <c r="N47" s="3"/>
+    </row>
+    <row r="48" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>47</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1.3073600000000001</v>
+      </c>
+      <c r="C48" s="3">
+        <v>103.854623</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E48" s="3">
+        <v>39</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M48" s="8">
+        <v>38749</v>
+      </c>
+      <c r="N48" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update on Feb 12
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="126">
   <si>
     <t>Male</t>
   </si>
@@ -341,6 +341,9 @@
     <t>Nationality</t>
   </si>
   <si>
+    <t>Cluster</t>
+  </si>
+  <si>
     <t>WhereInfected</t>
   </si>
   <si>
@@ -359,9 +362,6 @@
     <t>Bangladesh</t>
   </si>
   <si>
-    <t>Chinese (PR)</t>
-  </si>
-  <si>
     <t>Indonesian</t>
   </si>
   <si>
@@ -381,6 +381,45 @@
   </si>
   <si>
     <t>Johor Bahru, Resorts World Sentosa Casino, TTSH, NCID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PR</t>
+  </si>
+  <si>
+    <t>The Life Church and Missions Singapore</t>
+  </si>
+  <si>
+    <t>Yong Thai Hang</t>
+  </si>
+  <si>
+    <t>Grand Hyatt Singapore</t>
+  </si>
+  <si>
+    <t>Seletar Aerospace Heights construction site</t>
+  </si>
+  <si>
+    <t>Grace Assembly of God</t>
+  </si>
+  <si>
+    <t>Feb-11</t>
+  </si>
+  <si>
+    <t>Malaysia, Plaza Singapura, Star Vista, Fusionopolis, Grace Assembly of God (Tanglin), Grace Assembly of God (Bukit Batok), GP clinics, NCID</t>
+  </si>
+  <si>
+    <t>Bukit Batok Street 25</t>
+  </si>
+  <si>
+    <t>Grace Assembly of God (Tanglin), Grace Assembly of God (Bukit Batok), GP clinic, NUH emergency department</t>
+  </si>
+  <si>
+    <t>Toh Guan Road</t>
+  </si>
+  <si>
+    <t>DBS Asia Central at Marina Bay Financial Centre</t>
+  </si>
+  <si>
+    <t>Feb-12</t>
   </si>
 </sst>
 </file>
@@ -738,10 +777,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,7 +800,7 @@
     <col min="14" max="14" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
@@ -781,7 +820,7 @@
         <v>37</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>38</v>
@@ -799,13 +838,16 @@
         <v>98</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -836,14 +878,15 @@
       <c r="J2" s="4"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M2" s="8">
         <v>44562</v>
       </c>
       <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -876,14 +919,17 @@
         <v>96</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="M3" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="M3" s="8">
+        <v>44197</v>
+      </c>
       <c r="N3" s="8">
         <v>39114</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -916,14 +962,15 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M4" s="8">
         <v>44562</v>
       </c>
       <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -952,16 +999,21 @@
         <v>8</v>
       </c>
       <c r="J5" s="4"/>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="L5" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M5" s="8">
         <v>44562</v>
       </c>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="N5" s="8">
+        <v>40940</v>
+      </c>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -992,14 +1044,15 @@
       <c r="J6" s="4"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M6" s="8">
         <v>45292</v>
       </c>
       <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1030,14 +1083,15 @@
       <c r="J7" s="4"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M7" s="8">
         <v>45658</v>
       </c>
       <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1070,14 +1124,17 @@
         <v>96</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="M8" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="M8" s="8">
+        <v>45292</v>
+      </c>
       <c r="N8" s="8">
         <v>38018</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1108,14 +1165,17 @@
       <c r="J9" s="4"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M9" s="8">
         <v>43466</v>
       </c>
       <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O9" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1146,14 +1206,17 @@
       <c r="J10" s="4"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M10" s="8">
         <v>43466</v>
       </c>
       <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O10" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1188,14 +1251,17 @@
         <v>96</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="M11" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="M11" s="8">
+        <v>44197</v>
+      </c>
       <c r="N11" s="8">
         <v>39845</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1228,14 +1294,17 @@
         <v>96</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="M12" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="M12" s="8">
+        <v>46388</v>
+      </c>
       <c r="N12" s="8">
         <v>40210</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1264,16 +1333,21 @@
         <v>19</v>
       </c>
       <c r="J13" s="4"/>
-      <c r="K13" s="3"/>
+      <c r="K13" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="L13" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M13" s="8">
         <v>46023</v>
       </c>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="N13" s="8">
+        <v>40940</v>
+      </c>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1306,14 +1380,17 @@
         <v>96</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="M14" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="M14" s="8">
+        <v>46753</v>
+      </c>
       <c r="N14" s="8">
         <v>39845</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1344,14 +1421,15 @@
       <c r="J15" s="4"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M15" s="8">
         <v>46753</v>
       </c>
       <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1388,8 +1466,9 @@
         <v>10959</v>
       </c>
       <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1420,14 +1499,15 @@
       <c r="J17" s="4"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M17" s="8">
         <v>44562</v>
       </c>
       <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1466,8 +1546,9 @@
         <v>10959</v>
       </c>
       <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1498,14 +1579,15 @@
       <c r="J19" s="4"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M19" s="8">
         <v>36923</v>
       </c>
       <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1536,14 +1618,17 @@
       <c r="J20" s="4"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="M20" s="8">
         <v>47119</v>
       </c>
       <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O20" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1582,8 +1667,11 @@
         <v>45658</v>
       </c>
       <c r="N21" s="3"/>
-    </row>
-    <row r="22" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O21" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1618,10 +1706,15 @@
       <c r="L22" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="M22" s="3"/>
+      <c r="M22" s="8">
+        <v>37288</v>
+      </c>
       <c r="N22" s="3"/>
-    </row>
-    <row r="23" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O22" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1632,7 +1725,7 @@
         <v>103.99122566</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E23" s="3">
         <v>41</v>
@@ -1656,12 +1749,15 @@
       <c r="L23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M23" s="3"/>
+      <c r="M23" s="8">
+        <v>10959</v>
+      </c>
       <c r="N23" s="8">
         <v>39845</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1698,8 +1794,9 @@
         <v>10959</v>
       </c>
       <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1738,8 +1835,11 @@
         <v>10959</v>
       </c>
       <c r="N25" s="3"/>
-    </row>
-    <row r="26" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O25" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1770,16 +1870,23 @@
       <c r="J26" s="4">
         <v>24</v>
       </c>
-      <c r="K26" s="3"/>
+      <c r="K26" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="L26" s="3" t="s">
         <v>25</v>
       </c>
       <c r="M26" s="8">
         <v>45292</v>
       </c>
-      <c r="N26" s="3"/>
-    </row>
-    <row r="27" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="N26" s="8">
+        <v>40940</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -1814,14 +1921,17 @@
         <v>96</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="M27" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="M27" s="8">
+        <v>44197</v>
+      </c>
       <c r="N27" s="8">
         <v>39845</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1856,10 +1966,15 @@
       <c r="L28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M28" s="3"/>
+      <c r="M28" s="8">
+        <v>37288</v>
+      </c>
       <c r="N28" s="3"/>
-    </row>
-    <row r="29" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O28" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1894,10 +2009,15 @@
       <c r="L29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M29" s="3"/>
+      <c r="M29" s="8">
+        <v>37288</v>
+      </c>
       <c r="N29" s="3"/>
-    </row>
-    <row r="30" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O29" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1924,16 +2044,21 @@
         <v>58</v>
       </c>
       <c r="J30" s="4"/>
-      <c r="K30" s="3"/>
+      <c r="K30" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="L30" s="3" t="s">
         <v>25</v>
       </c>
       <c r="M30" s="8">
         <v>46753</v>
       </c>
-      <c r="N30" s="3"/>
-    </row>
-    <row r="31" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="N30" s="8">
+        <v>40940</v>
+      </c>
+      <c r="O30" s="3"/>
+    </row>
+    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -1968,8 +2093,11 @@
         <v>43831</v>
       </c>
       <c r="N31" s="3"/>
-    </row>
-    <row r="32" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O31" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2006,8 +2134,11 @@
         <v>44927</v>
       </c>
       <c r="N32" s="3"/>
-    </row>
-    <row r="33" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O32" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2040,10 +2171,13 @@
       <c r="L33" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M33" s="3"/>
+      <c r="M33" s="8">
+        <v>37288</v>
+      </c>
       <c r="N33" s="3"/>
-    </row>
-    <row r="34" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O33" s="3"/>
+    </row>
+    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2080,8 +2214,11 @@
         <v>10959</v>
       </c>
       <c r="N34" s="3"/>
-    </row>
-    <row r="35" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O34" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2112,16 +2249,23 @@
       <c r="J35" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K35" s="3"/>
+      <c r="K35" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="L35" s="3" t="s">
         <v>25</v>
       </c>
       <c r="M35" s="8">
         <v>46388</v>
       </c>
-      <c r="N35" s="3"/>
-    </row>
-    <row r="36" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="N35" s="8">
+        <v>40940</v>
+      </c>
+      <c r="O35" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2158,8 +2302,9 @@
         <v>11324</v>
       </c>
       <c r="N36" s="3"/>
-    </row>
-    <row r="37" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O36" s="3"/>
+    </row>
+    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -2192,14 +2337,17 @@
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M37" s="8">
         <v>45292</v>
       </c>
       <c r="N37" s="3"/>
-    </row>
-    <row r="38" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O37" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -2236,8 +2384,9 @@
         <v>10959</v>
       </c>
       <c r="N38" s="3"/>
-    </row>
-    <row r="39" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -2270,10 +2419,15 @@
       <c r="L39" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M39" s="3"/>
+      <c r="M39" s="8">
+        <v>37653</v>
+      </c>
       <c r="N39" s="3"/>
-    </row>
-    <row r="40" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O39" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -2312,8 +2466,11 @@
         <v>47119</v>
       </c>
       <c r="N40" s="3"/>
-    </row>
-    <row r="41" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O40" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -2344,16 +2501,23 @@
       <c r="J41" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K41" s="3"/>
+      <c r="K41" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="L41" s="3" t="s">
         <v>25</v>
       </c>
       <c r="M41" s="8">
         <v>10959</v>
       </c>
-      <c r="N41" s="3"/>
-    </row>
-    <row r="42" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="N41" s="8">
+        <v>40940</v>
+      </c>
+      <c r="O41" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -2390,8 +2554,9 @@
         <v>36923</v>
       </c>
       <c r="N42" s="3"/>
-    </row>
-    <row r="43" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O42" s="3"/>
+    </row>
+    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -2422,12 +2587,17 @@
       <c r="J43" s="4"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="M43" s="3"/>
+        <v>105</v>
+      </c>
+      <c r="M43" s="8">
+        <v>36923</v>
+      </c>
       <c r="N43" s="3"/>
-    </row>
-    <row r="44" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O43" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -2464,8 +2634,9 @@
         <v>10959</v>
       </c>
       <c r="N44" s="3"/>
-    </row>
-    <row r="45" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O44" s="3"/>
+    </row>
+    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -2498,10 +2669,13 @@
       <c r="L45" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M45" s="3"/>
+      <c r="M45" s="8">
+        <v>37288</v>
+      </c>
       <c r="N45" s="3"/>
-    </row>
-    <row r="46" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O45" s="3"/>
+    </row>
+    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -2538,8 +2712,9 @@
         <v>10959</v>
       </c>
       <c r="N46" s="3"/>
-    </row>
-    <row r="47" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O46" s="3"/>
+    </row>
+    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -2576,8 +2751,9 @@
         <v>38384</v>
       </c>
       <c r="N47" s="3"/>
-    </row>
-    <row r="48" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="O47" s="3"/>
+    </row>
+    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -2610,12 +2786,166 @@
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M48" s="8">
         <v>38749</v>
       </c>
       <c r="N48" s="3"/>
+      <c r="O48" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1.344174</v>
+      </c>
+      <c r="C49" s="3">
+        <v>103.760718</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E49" s="3">
+        <v>34</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J49" s="4"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M49" s="8">
+        <v>36923</v>
+      </c>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3">
+        <v>1.3370409999999999</v>
+      </c>
+      <c r="C50" s="3">
+        <v>103.74762699999999</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" s="3">
+        <v>46</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="J50" s="4"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M50" s="8">
+        <v>37653</v>
+      </c>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3">
+        <v>1.278713</v>
+      </c>
+      <c r="C51" s="3">
+        <v>103.85458199999999</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E51" s="3">
+        <v>62</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="J51" s="4"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+    </row>
+    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+    </row>
+    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update on Feb 13
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="144">
   <si>
     <t>Male</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Visited</t>
   </si>
   <si>
-    <t>Related</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -420,6 +417,63 @@
   </si>
   <si>
     <t>Feb-12</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>LinkedTo</t>
+  </si>
+  <si>
+    <t>Grace Assembly of God (Tanglin), Grace Assembly of God (Bukit Batok), GP clinic</t>
+  </si>
+  <si>
+    <t>Bishan Street 13</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>Seletar Aerospace Heights construction site, Tan Tock Seng Hospital</t>
+  </si>
+  <si>
+    <t>Campbell Lane</t>
+  </si>
+  <si>
+    <t>Hillview Avenue</t>
+  </si>
+  <si>
+    <t>National University of Singapore, Grace Assembly of God, NCID</t>
+  </si>
+  <si>
+    <t>Feb-13</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Mei Hwan Drive</t>
+  </si>
+  <si>
+    <t>Jan-22</t>
+  </si>
+  <si>
+    <t>Jan-21</t>
+  </si>
+  <si>
+    <t>Jan-19</t>
+  </si>
+  <si>
+    <t>Jan-26</t>
+  </si>
+  <si>
+    <t>Feb-02</t>
+  </si>
+  <si>
+    <t>Jan-20</t>
+  </si>
+  <si>
+    <t>27</t>
   </si>
 </sst>
 </file>
@@ -478,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -495,7 +549,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F11" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,8 +852,8 @@
     <col min="10" max="10" width="23.6640625" style="5" customWidth="1"/>
     <col min="11" max="11" width="15.5" customWidth="1"/>
     <col min="12" max="12" width="19.33203125" customWidth="1"/>
-    <col min="13" max="13" width="22.83203125" customWidth="1"/>
-    <col min="14" max="14" width="20.5" customWidth="1"/>
+    <col min="13" max="13" width="22.83203125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="20.5" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
@@ -811,7 +867,7 @@
         <v>41</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>42</v>
@@ -820,7 +876,7 @@
         <v>37</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>38</v>
@@ -829,22 +885,22 @@
         <v>43</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="L1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -858,7 +914,7 @@
         <v>103.80979619999999</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" s="3">
         <v>66</v>
@@ -878,12 +934,12 @@
       <c r="J2" s="4"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M2" s="8">
-        <v>44562</v>
-      </c>
-      <c r="N2" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="N2" s="8"/>
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -897,7 +953,7 @@
         <v>103.8585204</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="3">
         <v>53</v>
@@ -916,16 +972,16 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M3" s="8">
-        <v>44197</v>
-      </c>
-      <c r="N3" s="8">
-        <v>39114</v>
+        <v>102</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="O3" s="3"/>
     </row>
@@ -940,7 +996,7 @@
         <v>103.810018</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="3">
         <v>37</v>
@@ -962,12 +1018,12 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M4" s="8">
-        <v>44562</v>
-      </c>
-      <c r="N4" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="N4" s="8"/>
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -981,7 +1037,7 @@
         <v>103.820006847</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="3">
         <v>36</v>
@@ -1000,16 +1056,16 @@
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M5" s="8">
-        <v>44562</v>
-      </c>
-      <c r="N5" s="8">
-        <v>40940</v>
+        <v>102</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="O5" s="3"/>
     </row>
@@ -1024,7 +1080,7 @@
         <v>103.900929093</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="3">
         <v>56</v>
@@ -1044,12 +1100,12 @@
       <c r="J6" s="4"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M6" s="8">
-        <v>45292</v>
-      </c>
-      <c r="N6" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N6" s="8"/>
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1063,7 +1119,7 @@
         <v>103.944834173</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E7" s="3">
         <v>56</v>
@@ -1083,12 +1139,12 @@
       <c r="J7" s="4"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M7" s="8">
-        <v>45658</v>
-      </c>
-      <c r="N7" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N7" s="8"/>
       <c r="O7" s="3"/>
     </row>
     <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1102,7 +1158,7 @@
         <v>103.860577941</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="3">
         <v>35</v>
@@ -1121,16 +1177,16 @@
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M8" s="8">
-        <v>45292</v>
-      </c>
-      <c r="N8" s="8">
-        <v>38018</v>
+        <v>102</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="O8" s="3"/>
     </row>
@@ -1145,7 +1201,7 @@
         <v>103.87764483700001</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9" s="3">
         <v>56</v>
@@ -1165,14 +1221,14 @@
       <c r="J9" s="4"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M9" s="8">
-        <v>43466</v>
-      </c>
-      <c r="N9" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="N9" s="8"/>
       <c r="O9" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1186,7 +1242,7 @@
         <v>103.87756705300001</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="3">
         <v>56</v>
@@ -1206,14 +1262,14 @@
       <c r="J10" s="4"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M10" s="8">
-        <v>43466</v>
-      </c>
-      <c r="N10" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="N10" s="8"/>
       <c r="O10" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1227,7 +1283,7 @@
         <v>103.8631688</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="3">
         <v>56</v>
@@ -1248,16 +1304,16 @@
         <v>4</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M11" s="8">
-        <v>44197</v>
-      </c>
-      <c r="N11" s="8">
-        <v>39845</v>
+        <v>102</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="O11" s="3"/>
     </row>
@@ -1272,7 +1328,7 @@
         <v>103.820199966</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12" s="3">
         <v>31</v>
@@ -1291,16 +1347,16 @@
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M12" s="8">
-        <v>46388</v>
-      </c>
-      <c r="N12" s="8">
-        <v>40210</v>
+        <v>102</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="O12" s="3"/>
     </row>
@@ -1315,7 +1371,7 @@
         <v>103.819829822</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" s="3">
         <v>37</v>
@@ -1334,16 +1390,16 @@
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M13" s="8">
-        <v>46023</v>
-      </c>
-      <c r="N13" s="8">
-        <v>40940</v>
+        <v>102</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="O13" s="3"/>
     </row>
@@ -1358,7 +1414,7 @@
         <v>103.846496344</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E14" s="3">
         <v>73</v>
@@ -1377,16 +1433,16 @@
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M14" s="8">
-        <v>46753</v>
-      </c>
-      <c r="N14" s="8">
-        <v>39845</v>
+        <v>102</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="O14" s="3"/>
     </row>
@@ -1401,7 +1457,7 @@
         <v>103.737467229</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="3">
         <v>31</v>
@@ -1421,12 +1477,12 @@
       <c r="J15" s="4"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M15" s="8">
-        <v>46753</v>
-      </c>
-      <c r="N15" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="N15" s="8"/>
       <c r="O15" s="3"/>
     </row>
     <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1440,7 +1496,7 @@
         <v>103.99087428999999</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16" s="3">
         <v>47</v>
@@ -1452,7 +1508,7 @@
         <v>25</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>1</v>
@@ -1462,10 +1518,10 @@
       <c r="L16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M16" s="8">
-        <v>10959</v>
-      </c>
-      <c r="N16" s="3"/>
+      <c r="M16" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N16" s="8"/>
       <c r="O16" s="3"/>
     </row>
     <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1479,7 +1535,7 @@
         <v>103.8256719</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="3">
         <v>38</v>
@@ -1499,12 +1555,12 @@
       <c r="J17" s="4"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M17" s="8">
-        <v>44562</v>
-      </c>
-      <c r="N17" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="N17" s="8"/>
       <c r="O17" s="3"/>
     </row>
     <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1518,7 +1574,7 @@
         <v>103.991131783</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" s="3">
         <v>47</v>
@@ -1530,7 +1586,7 @@
         <v>25</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>1</v>
@@ -1539,16 +1595,16 @@
         <v>12</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M18" s="8">
-        <v>10959</v>
-      </c>
-      <c r="N18" s="8">
-        <v>40575</v>
+      <c r="M18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="O18" s="3"/>
     </row>
@@ -1563,7 +1619,7 @@
         <v>103.878130317</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" s="3">
         <v>31</v>
@@ -1583,12 +1639,12 @@
       <c r="J19" s="4"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M19" s="8">
-        <v>36923</v>
-      </c>
-      <c r="N19" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="N19" s="8"/>
       <c r="O19" s="3"/>
     </row>
     <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1602,7 +1658,7 @@
         <v>103.81527811300001</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" s="3">
         <v>28</v>
@@ -1622,14 +1678,14 @@
       <c r="J20" s="4"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="M20" s="8">
-        <v>47119</v>
-      </c>
-      <c r="N20" s="3"/>
+        <v>112</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="N20" s="8"/>
       <c r="O20" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1643,7 +1699,7 @@
         <v>103.885970414</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" s="3">
         <v>48</v>
@@ -1667,12 +1723,12 @@
       <c r="L21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M21" s="8">
-        <v>45658</v>
-      </c>
-      <c r="N21" s="3"/>
+      <c r="M21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N21" s="8"/>
       <c r="O21" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1686,7 +1742,7 @@
         <v>103.815087676</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E22" s="3">
         <v>44</v>
@@ -1708,14 +1764,14 @@
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="M22" s="8">
-        <v>37288</v>
-      </c>
-      <c r="N22" s="3"/>
+        <v>105</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="N22" s="8"/>
       <c r="O22" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1729,7 +1785,7 @@
         <v>103.99122566</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E23" s="3">
         <v>41</v>
@@ -1741,23 +1797,23 @@
         <v>25</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M23" s="8">
-        <v>10959</v>
-      </c>
-      <c r="N23" s="8">
-        <v>39845</v>
+      <c r="M23" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="O23" s="3"/>
     </row>
@@ -1772,7 +1828,7 @@
         <v>103.99096548599999</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E24" s="3">
         <v>17</v>
@@ -1784,7 +1840,7 @@
         <v>25</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>1</v>
@@ -1794,10 +1850,10 @@
       <c r="L24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M24" s="8">
-        <v>10959</v>
-      </c>
-      <c r="N24" s="3"/>
+      <c r="M24" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N24" s="8"/>
       <c r="O24" s="3"/>
     </row>
     <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1811,7 +1867,7 @@
         <v>103.8826748</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E25" s="3">
         <v>32</v>
@@ -1835,12 +1891,12 @@
       <c r="L25" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M25" s="8">
-        <v>10959</v>
-      </c>
-      <c r="N25" s="3"/>
+      <c r="M25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N25" s="8"/>
       <c r="O25" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1854,7 +1910,7 @@
         <v>103.882692754</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E26" s="3">
         <v>32</v>
@@ -1875,19 +1931,19 @@
         <v>24</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M26" s="8">
-        <v>45292</v>
-      </c>
-      <c r="N26" s="8">
-        <v>40940</v>
+      <c r="M26" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N26" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1901,7 +1957,7 @@
         <v>103.847638965</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E27" s="3">
         <v>42</v>
@@ -1922,16 +1978,16 @@
         <v>13</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="M27" s="8">
-        <v>44197</v>
-      </c>
-      <c r="N27" s="8">
-        <v>39845</v>
+        <v>102</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="N27" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="O27" s="3"/>
     </row>
@@ -1946,7 +2002,7 @@
         <v>103.81559461400001</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E28" s="3">
         <v>45</v>
@@ -1970,12 +2026,12 @@
       <c r="L28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M28" s="8">
-        <v>37288</v>
-      </c>
-      <c r="N28" s="3"/>
+      <c r="M28" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="N28" s="8"/>
       <c r="O28" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -1989,7 +2045,7 @@
         <v>103.815433681</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E29" s="3">
         <v>0.6</v>
@@ -2006,19 +2062,19 @@
       <c r="I29" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J29" s="4">
-        <v>27</v>
+      <c r="J29" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M29" s="8">
-        <v>37288</v>
-      </c>
-      <c r="N29" s="3"/>
+      <c r="M29" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="N29" s="8"/>
       <c r="O29" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2032,7 +2088,7 @@
         <v>103.84413499999999</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E30" s="3">
         <v>41</v>
@@ -2045,20 +2101,20 @@
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L30" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M30" s="8">
-        <v>46753</v>
-      </c>
-      <c r="N30" s="8">
-        <v>40940</v>
+      <c r="M30" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="N30" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="O30" s="3"/>
     </row>
@@ -2073,7 +2129,7 @@
         <v>103.833184</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E31" s="3">
         <v>27</v>
@@ -2086,19 +2142,19 @@
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M31" s="8">
-        <v>43831</v>
-      </c>
-      <c r="N31" s="3"/>
+      <c r="M31" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="N31" s="8"/>
       <c r="O31" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2112,7 +2168,7 @@
         <v>103.95156299999999</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E32" s="3">
         <v>53</v>
@@ -2124,22 +2180,22 @@
         <v>25</v>
       </c>
       <c r="H32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I32" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M32" s="8">
-        <v>44927</v>
-      </c>
-      <c r="N32" s="3"/>
+      <c r="M32" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N32" s="8"/>
       <c r="O32" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2153,7 +2209,7 @@
         <v>103.94172</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E33" s="3">
         <v>42</v>
@@ -2165,20 +2221,20 @@
         <v>25</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M33" s="8">
-        <v>37288</v>
-      </c>
-      <c r="N33" s="3"/>
+      <c r="M33" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="N33" s="8"/>
       <c r="O33" s="3"/>
     </row>
     <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2192,7 +2248,7 @@
         <v>103.894414</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E34" s="3">
         <v>39</v>
@@ -2204,22 +2260,22 @@
         <v>25</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M34" s="8">
-        <v>10959</v>
-      </c>
-      <c r="N34" s="3"/>
+      <c r="M34" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N34" s="8"/>
       <c r="O34" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2233,7 +2289,7 @@
         <v>103.838301</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E35" s="3">
         <v>40</v>
@@ -2245,28 +2301,28 @@
         <v>25</v>
       </c>
       <c r="H35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I35" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="I35" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="J35" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L35" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M35" s="8">
-        <v>46388</v>
-      </c>
-      <c r="N35" s="8">
-        <v>40940</v>
+      <c r="M35" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="N35" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2280,7 +2336,7 @@
         <v>103.821619</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E36" s="3">
         <v>64</v>
@@ -2292,20 +2348,20 @@
         <v>25</v>
       </c>
       <c r="H36" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M36" s="8">
-        <v>11324</v>
-      </c>
-      <c r="N36" s="3"/>
+      <c r="M36" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N36" s="8"/>
       <c r="O36" s="3"/>
     </row>
     <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2319,7 +2375,7 @@
         <v>103.75111699999999</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E37" s="3">
         <v>38</v>
@@ -2331,28 +2387,28 @@
         <v>25</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M37" s="8">
-        <v>45292</v>
-      </c>
-      <c r="N37" s="8">
-        <v>40575</v>
+        <v>106</v>
+      </c>
+      <c r="M37" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N37" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2366,7 +2422,7 @@
         <v>103.73366300000001</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E38" s="3">
         <v>53</v>
@@ -2378,20 +2434,20 @@
         <v>25</v>
       </c>
       <c r="H38" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M38" s="8">
-        <v>10959</v>
-      </c>
-      <c r="N38" s="3"/>
+      <c r="M38" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N38" s="8"/>
       <c r="O38" s="3"/>
     </row>
     <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2405,7 +2461,7 @@
         <v>103.741224</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E39" s="3">
         <v>52</v>
@@ -2417,22 +2473,22 @@
         <v>25</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M39" s="8">
-        <v>37653</v>
-      </c>
-      <c r="N39" s="3"/>
+      <c r="M39" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="N39" s="8"/>
       <c r="O39" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2446,7 +2502,7 @@
         <v>103.705433</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E40" s="3">
         <v>51</v>
@@ -2458,24 +2514,24 @@
         <v>25</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K40" s="3"/>
       <c r="L40" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M40" s="8">
-        <v>47119</v>
-      </c>
-      <c r="N40" s="3"/>
+      <c r="M40" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="N40" s="8"/>
       <c r="O40" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2489,7 +2545,7 @@
         <v>103.926856</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E41" s="3">
         <v>36</v>
@@ -2501,28 +2557,28 @@
         <v>25</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L41" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M41" s="8">
-        <v>10959</v>
-      </c>
-      <c r="N41" s="8">
-        <v>40940</v>
+      <c r="M41" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N41" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2536,7 +2592,7 @@
         <v>103.878049</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E42" s="3">
         <v>71</v>
@@ -2548,20 +2604,20 @@
         <v>25</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M42" s="8">
-        <v>36923</v>
-      </c>
-      <c r="N42" s="3"/>
+      <c r="M42" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="N42" s="8"/>
       <c r="O42" s="3"/>
     </row>
     <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2575,7 +2631,7 @@
         <v>103.910634</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E43" s="3">
         <v>39</v>
@@ -2587,22 +2643,22 @@
         <v>25</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="M43" s="8">
-        <v>36923</v>
-      </c>
-      <c r="N43" s="3"/>
+        <v>104</v>
+      </c>
+      <c r="M43" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="N43" s="8"/>
       <c r="O43" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2616,7 +2672,7 @@
         <v>103.880578</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E44" s="3">
         <v>54</v>
@@ -2628,20 +2684,20 @@
         <v>25</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M44" s="8">
-        <v>10959</v>
-      </c>
-      <c r="N44" s="3"/>
+      <c r="M44" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N44" s="8"/>
       <c r="O44" s="3"/>
     </row>
     <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2655,7 +2711,7 @@
         <v>103.816625</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E45" s="3">
         <v>37</v>
@@ -2667,20 +2723,22 @@
         <v>25</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="J45" s="4"/>
+        <v>91</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="K45" s="3"/>
       <c r="L45" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M45" s="8">
-        <v>37288</v>
-      </c>
-      <c r="N45" s="3"/>
+      <c r="M45" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="N45" s="8"/>
       <c r="O45" s="3"/>
     </row>
     <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2694,7 +2752,7 @@
         <v>103.84683800000001</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E46" s="3">
         <v>2</v>
@@ -2706,20 +2764,20 @@
         <v>1</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="3"/>
       <c r="L46" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M46" s="8">
-        <v>10959</v>
-      </c>
-      <c r="N46" s="3"/>
+      <c r="M46" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N46" s="8"/>
       <c r="O46" s="3"/>
     </row>
     <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2733,7 +2791,7 @@
         <v>103.82021400000001</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E47" s="3">
         <v>35</v>
@@ -2745,20 +2803,20 @@
         <v>25</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J47" s="4"/>
       <c r="K47" s="3"/>
       <c r="L47" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="M47" s="8">
-        <v>38384</v>
-      </c>
-      <c r="N47" s="3"/>
+        <v>106</v>
+      </c>
+      <c r="M47" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="N47" s="8"/>
       <c r="O47" s="3"/>
     </row>
     <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2772,7 +2830,7 @@
         <v>103.854623</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E48" s="3">
         <v>39</v>
@@ -2784,24 +2842,24 @@
         <v>25</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="M48" s="8">
-        <v>38749</v>
-      </c>
-      <c r="N48" s="3"/>
+        <v>104</v>
+      </c>
+      <c r="M48" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="N48" s="8"/>
       <c r="O48" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2815,7 +2873,7 @@
         <v>103.760718</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E49" s="3">
         <v>34</v>
@@ -2827,22 +2885,22 @@
         <v>25</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J49" s="4"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M49" s="8">
-        <v>36923</v>
-      </c>
-      <c r="N49" s="3"/>
+      <c r="M49" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="N49" s="8"/>
       <c r="O49" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2856,7 +2914,7 @@
         <v>103.74762699999999</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E50" s="3">
         <v>46</v>
@@ -2868,22 +2926,22 @@
         <v>25</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M50" s="8">
-        <v>37653</v>
-      </c>
-      <c r="N50" s="3"/>
+      <c r="M50" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="N50" s="8"/>
       <c r="O50" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -2897,7 +2955,7 @@
         <v>103.85458199999999</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E51" s="3">
         <v>62</v>
@@ -2908,52 +2966,334 @@
       <c r="G51" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H51" s="3"/>
+      <c r="H51" s="3" t="s">
+        <v>136</v>
+      </c>
       <c r="I51" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="3"/>
       <c r="L51" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
+      <c r="M51" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N51" s="8"/>
       <c r="O51" s="3"/>
     </row>
     <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
+      <c r="A52" s="3">
+        <v>51</v>
+      </c>
+      <c r="B52" s="3">
+        <v>1.349558</v>
+      </c>
+      <c r="C52" s="3">
+        <v>103.85372099999999</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E52" s="3">
+        <v>48</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="J52" s="4"/>
       <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
+      <c r="L52" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M52" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N52" s="8"/>
+      <c r="O52" s="3" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="4"/>
+      <c r="A53" s="3">
+        <v>52</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1.3055669999999999</v>
+      </c>
+      <c r="C53" s="3">
+        <v>103.85220700000001</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E53" s="3">
+        <v>37</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="3"/>
-      <c r="O53" s="3"/>
+      <c r="L53" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M53" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N53" s="8"/>
+      <c r="O53" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>53</v>
+      </c>
+      <c r="B54" s="3">
+        <v>1.3597619999999999</v>
+      </c>
+      <c r="C54" s="3">
+        <v>103.764067</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E54" s="3">
+        <v>54</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="J54" s="4"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M54" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="N54" s="8"/>
+      <c r="O54" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>54</v>
+      </c>
+      <c r="B55" s="3">
+        <v>1.2942720000000001</v>
+      </c>
+      <c r="C55" s="3">
+        <v>103.816311</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E55" s="3">
+        <v>54</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J55" s="4"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M55" s="8"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1.3538140000000001</v>
+      </c>
+      <c r="C56" s="3">
+        <v>103.860564</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" s="3">
+        <v>30</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I56" s="3"/>
+      <c r="J56" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="3"/>
+    </row>
+    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>56</v>
+      </c>
+      <c r="B57" s="3">
+        <v>1.4058390000000001</v>
+      </c>
+      <c r="C57" s="3">
+        <v>103.86582300000001</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E57" s="3">
+        <v>30</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J57" s="4"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M57" s="8"/>
+      <c r="N57" s="8"/>
+      <c r="O57" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>57</v>
+      </c>
+      <c r="B58" s="3">
+        <v>1.2942549999999999</v>
+      </c>
+      <c r="C58" s="3">
+        <v>103.816506</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E58" s="3">
+        <v>26</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J58" s="4"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>58</v>
+      </c>
+      <c r="B59" s="3">
+        <v>1.2945230000000001</v>
+      </c>
+      <c r="C59" s="3">
+        <v>103.816479</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E59" s="3">
+        <v>55</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J59" s="4"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M59" s="8"/>
+      <c r="N59" s="8"/>
+      <c r="O59" s="3" t="s">
+        <v>117</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update on Feb 14
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="160">
   <si>
     <t>Male</t>
   </si>
@@ -474,6 +474,54 @@
   </si>
   <si>
     <t>27</t>
+  </si>
+  <si>
+    <t>Feb-14</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>Farrer Park Hospital’s emergency care clinic, Mount Elizabeth Hospital emergency department</t>
+  </si>
+  <si>
+    <t>Wilkinson Road</t>
+  </si>
+  <si>
+    <t>Ang Mo Kio Avenue 3</t>
+  </si>
+  <si>
+    <t>Grace Assembly of God (Tanglin), GP Clinic</t>
+  </si>
+  <si>
+    <t>Jurong West Street 64</t>
+  </si>
+  <si>
+    <t>Grace Assembly of God, Legacy Office Supplies Pte Ltd (56 Senang Crescent), GP clinic, Ng Teng Fong General Hospital, Pioneer Polyclinic, National University Hospital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grace Assembly of God, GP clinic, Singapore General Hospital </t>
+  </si>
+  <si>
+    <t>Tanjong Pagar Road</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>Grace Assembly of God (Tanglin)</t>
+  </si>
+  <si>
+    <t>Ang Mo Kio Avenue 5</t>
+  </si>
+  <si>
+    <t>Pulau Bukom, Church of Christ the King (2221 Ang Mo Kio Avenue 8), GP Clinic</t>
+  </si>
+  <si>
+    <t>Senja Road</t>
+  </si>
+  <si>
+    <t>Jalan Kelichap</t>
   </si>
 </sst>
 </file>
@@ -833,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2145,14 +2193,18 @@
         <v>58</v>
       </c>
       <c r="J31" s="4"/>
-      <c r="K31" s="3"/>
+      <c r="K31" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L31" s="3" t="s">
         <v>25</v>
       </c>
       <c r="M31" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="N31" s="8"/>
+      <c r="N31" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="O31" s="3" t="s">
         <v>115</v>
       </c>
@@ -2770,14 +2822,18 @@
         <v>93</v>
       </c>
       <c r="J46" s="4"/>
-      <c r="K46" s="3"/>
+      <c r="K46" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L46" s="3" t="s">
         <v>25</v>
       </c>
       <c r="M46" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="N46" s="8"/>
+      <c r="N46" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="O46" s="3"/>
     </row>
     <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -3113,16 +3169,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="3">
-        <v>1.2942720000000001</v>
+        <v>1.375907</v>
       </c>
       <c r="C55" s="3">
-        <v>103.816311</v>
+        <v>103.854193</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>134</v>
       </c>
       <c r="E55" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>4</v>
@@ -3130,16 +3186,20 @@
       <c r="G55" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H55" s="3"/>
+      <c r="H55" s="3" t="s">
+        <v>156</v>
+      </c>
       <c r="I55" s="3" t="s">
-        <v>117</v>
+        <v>155</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M55" s="8"/>
+      <c r="M55" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="N55" s="8"/>
       <c r="O55" s="3" t="s">
         <v>117</v>
@@ -3170,7 +3230,9 @@
       <c r="H56" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="I56" s="3"/>
+      <c r="I56" s="3" t="s">
+        <v>157</v>
+      </c>
       <c r="J56" s="4" t="s">
         <v>135</v>
       </c>
@@ -3178,7 +3240,9 @@
       <c r="L56" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M56" s="8"/>
+      <c r="M56" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="N56" s="8"/>
       <c r="O56" s="3"/>
     </row>
@@ -3208,14 +3272,18 @@
         <v>116</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="J57" s="4"/>
+        <v>130</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="K57" s="3"/>
       <c r="L57" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="M57" s="8"/>
+      <c r="M57" s="8" t="s">
+        <v>124</v>
+      </c>
       <c r="N57" s="8"/>
       <c r="O57" s="3" t="s">
         <v>116</v>
@@ -3226,10 +3294,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="3">
-        <v>1.2942549999999999</v>
+        <v>1.3868290000000001</v>
       </c>
       <c r="C58" s="3">
-        <v>103.816506</v>
+        <v>103.761758</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>134</v>
@@ -3243,7 +3311,9 @@
       <c r="G58" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H58" s="3"/>
+      <c r="H58" s="3" t="s">
+        <v>158</v>
+      </c>
       <c r="I58" s="3" t="s">
         <v>117</v>
       </c>
@@ -3252,7 +3322,9 @@
       <c r="L58" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M58" s="8"/>
+      <c r="M58" s="8" t="s">
+        <v>118</v>
+      </c>
       <c r="N58" s="8"/>
       <c r="O58" s="3" t="s">
         <v>117</v>
@@ -3263,10 +3335,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="3">
-        <v>1.2945230000000001</v>
+        <v>1.3467119999999999</v>
       </c>
       <c r="C59" s="3">
-        <v>103.816479</v>
+        <v>103.88141899999999</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>134</v>
@@ -3280,7 +3352,9 @@
       <c r="G59" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H59" s="3"/>
+      <c r="H59" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="I59" s="3" t="s">
         <v>117</v>
       </c>
@@ -3289,11 +3363,366 @@
       <c r="L59" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="M59" s="8"/>
+      <c r="M59" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="N59" s="8"/>
       <c r="O59" s="3" t="s">
         <v>117</v>
       </c>
+    </row>
+    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3">
+        <v>1.302775</v>
+      </c>
+      <c r="C60" s="3">
+        <v>103.891108</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E60" s="3">
+        <v>61</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="J60" s="4"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M60" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N60" s="8"/>
+      <c r="O60" s="3"/>
+    </row>
+    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>60</v>
+      </c>
+      <c r="B61" s="3">
+        <v>1.369327</v>
+      </c>
+      <c r="C61" s="3">
+        <v>103.85627599999999</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E61" s="3">
+        <v>51</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="J61" s="4"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M61" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="N61" s="8"/>
+      <c r="O61" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>61</v>
+      </c>
+      <c r="B62" s="3">
+        <v>1.341642</v>
+      </c>
+      <c r="C62" s="3">
+        <v>103.70378700000001</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E62" s="3">
+        <v>57</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J62" s="4"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M62" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="N62" s="8"/>
+      <c r="O62" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>62</v>
+      </c>
+      <c r="B63" s="3">
+        <v>1.2763329999999999</v>
+      </c>
+      <c r="C63" s="3">
+        <v>103.843384</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E63" s="3">
+        <v>44</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J63" s="4"/>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M63" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N63" s="8"/>
+      <c r="O63" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>63</v>
+      </c>
+      <c r="B64" s="3">
+        <v>1.2942899999999999</v>
+      </c>
+      <c r="C64" s="3">
+        <v>103.81654899999999</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E64" s="3">
+        <v>54</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J64" s="4"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M64" s="8"/>
+      <c r="N64" s="8"/>
+      <c r="O64" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <v>64</v>
+      </c>
+      <c r="B65" s="3">
+        <v>1.3220970000000001</v>
+      </c>
+      <c r="C65" s="3">
+        <v>103.847273</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E65" s="3">
+        <v>50</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M65" s="8"/>
+      <c r="N65" s="8"/>
+      <c r="O65" s="3"/>
+    </row>
+    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>65</v>
+      </c>
+      <c r="B66" s="3">
+        <v>1.353793</v>
+      </c>
+      <c r="C66" s="3">
+        <v>103.86065000000001</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E66" s="3">
+        <v>61</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I66" s="3"/>
+      <c r="J66" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M66" s="8"/>
+      <c r="N66" s="8"/>
+      <c r="O66" s="3"/>
+    </row>
+    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>66</v>
+      </c>
+      <c r="B67" s="3">
+        <v>1.294427</v>
+      </c>
+      <c r="C67" s="3">
+        <v>103.816418</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E67" s="3">
+        <v>28</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J67" s="4"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M67" s="8"/>
+      <c r="N67" s="8"/>
+      <c r="O67" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
+        <v>67</v>
+      </c>
+      <c r="B68" s="3">
+        <v>1.3405910000000001</v>
+      </c>
+      <c r="C68" s="3">
+        <v>103.703937</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E68" s="3">
+        <v>56</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M68" s="8"/>
+      <c r="N68" s="8"/>
+      <c r="O68" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+    </row>
+    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update data on Feb 15
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="191">
   <si>
     <t>Male</t>
   </si>
@@ -476,9 +476,6 @@
     <t>Feb-14</t>
   </si>
   <si>
-    <t>55</t>
-  </si>
-  <si>
     <t>Farrer Park Hospital’s emergency care clinic, Mount Elizabeth Hospital emergency department</t>
   </si>
   <si>
@@ -522,6 +519,102 @@
   </si>
   <si>
     <t>Hillionton Green</t>
+  </si>
+  <si>
+    <t>Feb-15</t>
+  </si>
+  <si>
+    <t>50, 55</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>66, 70</t>
+  </si>
+  <si>
+    <t>66, 68</t>
+  </si>
+  <si>
+    <t>68, 70</t>
+  </si>
+  <si>
+    <t>Grace Assembly of God, PUB, Marisson Hotel Bugis (103 Beach Road)</t>
+  </si>
+  <si>
+    <t>Potong Pasir Avenue 3</t>
+  </si>
+  <si>
+    <t>NUH</t>
+  </si>
+  <si>
+    <t>GP clinics, NUH</t>
+  </si>
+  <si>
+    <t>Jurong West Street 81</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>Taxi Driver</t>
+  </si>
+  <si>
+    <t>Church of Christ the King (2221 Ang Mo Kio Avenue 8)</t>
+  </si>
+  <si>
+    <t>NCID</t>
+  </si>
+  <si>
+    <t>Grace Assembly of God, God’s Kingdom Bread of Life Church (37 Jalan Permimpin)</t>
+  </si>
+  <si>
+    <t>Grace Assembly of God (Bukit Batok), Ng Teng Fong General Hospital, NUH</t>
+  </si>
+  <si>
+    <t>Singapore Work Pass holder</t>
+  </si>
+  <si>
+    <t>Tour Guide</t>
+  </si>
+  <si>
+    <t>Singapore Work Pass holder</t>
+  </si>
+  <si>
+    <t>Anaesthesiologist</t>
+  </si>
+  <si>
+    <t>NUS Professor</t>
+  </si>
+  <si>
+    <t>Private-Hire Driver</t>
+  </si>
+  <si>
+    <t>DBS employee</t>
+  </si>
+  <si>
+    <t>Singaporean</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
 </sst>
 </file>
@@ -881,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="C51" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -902,9 +995,10 @@
     <col min="12" max="12" width="19.33203125" customWidth="1"/>
     <col min="13" max="13" width="22.83203125" style="10" customWidth="1"/>
     <col min="14" max="14" width="20.5" style="10" customWidth="1"/>
+    <col min="15" max="16" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
@@ -950,8 +1044,11 @@
       <c r="O1" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P1" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -989,8 +1086,9 @@
       </c>
       <c r="N2" s="8"/>
       <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1032,8 +1130,9 @@
         <v>59</v>
       </c>
       <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1061,8 +1160,8 @@
       <c r="I4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="4">
-        <v>1</v>
+      <c r="J4" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
@@ -1073,8 +1172,9 @@
       </c>
       <c r="N4" s="8"/>
       <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1116,8 +1216,9 @@
         <v>124</v>
       </c>
       <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1155,8 +1256,9 @@
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1194,8 +1296,9 @@
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1237,8 +1340,9 @@
         <v>54</v>
       </c>
       <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1278,8 +1382,9 @@
       <c r="O9" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1319,8 +1424,9 @@
       <c r="O10" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1348,8 +1454,8 @@
       <c r="I11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="4">
-        <v>4</v>
+      <c r="J11" s="4" t="s">
+        <v>187</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>95</v>
@@ -1364,8 +1470,9 @@
         <v>90</v>
       </c>
       <c r="O11" s="3"/>
-    </row>
-    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1407,8 +1514,9 @@
         <v>94</v>
       </c>
       <c r="O12" s="3"/>
-    </row>
-    <row r="13" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1450,8 +1558,9 @@
         <v>124</v>
       </c>
       <c r="O13" s="3"/>
-    </row>
-    <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1493,8 +1602,9 @@
         <v>90</v>
       </c>
       <c r="O14" s="3"/>
-    </row>
-    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1532,8 +1642,9 @@
       </c>
       <c r="N15" s="8"/>
       <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1564,15 +1675,16 @@
       <c r="J16" s="4"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M16" s="8" t="s">
         <v>51</v>
       </c>
       <c r="N16" s="8"/>
       <c r="O16" s="3"/>
-    </row>
-    <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P16" s="3"/>
+    </row>
+    <row r="17" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1610,8 +1722,9 @@
       </c>
       <c r="N17" s="8"/>
       <c r="O17" s="3"/>
-    </row>
-    <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1639,14 +1752,14 @@
       <c r="I18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="4">
-        <v>12</v>
+      <c r="J18" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>95</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M18" s="8" t="s">
         <v>51</v>
@@ -1655,8 +1768,9 @@
         <v>118</v>
       </c>
       <c r="O18" s="3"/>
-    </row>
-    <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1694,8 +1808,9 @@
       </c>
       <c r="N19" s="8"/>
       <c r="O19" s="3"/>
-    </row>
-    <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1735,8 +1850,9 @@
       <c r="O20" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1764,12 +1880,12 @@
       <c r="I21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="4">
-        <v>19</v>
+      <c r="J21" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M21" s="8" t="s">
         <v>47</v>
@@ -1778,8 +1894,9 @@
       <c r="O21" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P21" s="3"/>
+    </row>
+    <row r="22" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1807,8 +1924,8 @@
       <c r="I22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J22" s="4">
-        <v>19</v>
+      <c r="J22" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3" t="s">
@@ -1821,8 +1938,9 @@
       <c r="O22" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1855,7 +1973,7 @@
         <v>95</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M23" s="8" t="s">
         <v>51</v>
@@ -1864,8 +1982,9 @@
         <v>90</v>
       </c>
       <c r="O23" s="3"/>
-    </row>
-    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P23" s="3"/>
+    </row>
+    <row r="24" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1896,15 +2015,16 @@
       <c r="J24" s="4"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M24" s="8" t="s">
         <v>51</v>
       </c>
       <c r="N24" s="8"/>
       <c r="O24" s="3"/>
-    </row>
-    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P24" s="3"/>
+    </row>
+    <row r="25" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1932,22 +2052,29 @@
       <c r="I25" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J25" s="4">
-        <v>19</v>
-      </c>
-      <c r="K25" s="3"/>
+      <c r="J25" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L25" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M25" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="N25" s="8"/>
+      <c r="N25" s="8" t="s">
+        <v>159</v>
+      </c>
       <c r="O25" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P25" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1975,14 +2102,14 @@
       <c r="I26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J26" s="4">
-        <v>24</v>
+      <c r="J26" s="4" t="s">
+        <v>189</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>95</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M26" s="8" t="s">
         <v>46</v>
@@ -1993,8 +2120,9 @@
       <c r="O26" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2022,8 +2150,8 @@
       <c r="I27" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J27" s="4">
-        <v>13</v>
+      <c r="J27" s="4" t="s">
+        <v>190</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>95</v>
@@ -2038,8 +2166,9 @@
         <v>90</v>
       </c>
       <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2067,12 +2196,12 @@
       <c r="I28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J28" s="4">
-        <v>19</v>
+      <c r="J28" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M28" s="8" t="s">
         <v>140</v>
@@ -2081,8 +2210,11 @@
       <c r="O28" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P28" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2115,7 +2247,7 @@
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M29" s="8" t="s">
         <v>140</v>
@@ -2124,8 +2256,9 @@
       <c r="O29" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P29" s="3"/>
+    </row>
+    <row r="30" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2156,7 +2289,7 @@
         <v>95</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M30" s="8" t="s">
         <v>49</v>
@@ -2165,8 +2298,9 @@
         <v>124</v>
       </c>
       <c r="O30" s="3"/>
-    </row>
-    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2197,7 +2331,7 @@
         <v>95</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M31" s="8" t="s">
         <v>141</v>
@@ -2208,8 +2342,9 @@
       <c r="O31" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P31" s="3"/>
+    </row>
+    <row r="32" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2240,7 +2375,7 @@
       <c r="J32" s="4"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M32" s="8" t="s">
         <v>45</v>
@@ -2249,8 +2384,9 @@
       <c r="O32" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2281,15 +2417,16 @@
       <c r="J33" s="4"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M33" s="8" t="s">
         <v>140</v>
       </c>
       <c r="N33" s="8"/>
       <c r="O33" s="3"/>
-    </row>
-    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2320,7 +2457,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M34" s="8" t="s">
         <v>51</v>
@@ -2329,8 +2466,9 @@
       <c r="O34" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P34" s="3"/>
+    </row>
+    <row r="35" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2365,7 +2503,7 @@
         <v>95</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M35" s="8" t="s">
         <v>48</v>
@@ -2376,8 +2514,9 @@
       <c r="O35" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P35" s="3"/>
+    </row>
+    <row r="36" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2408,15 +2547,16 @@
       <c r="J36" s="4"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M36" s="8" t="s">
         <v>52</v>
       </c>
       <c r="N36" s="8"/>
       <c r="O36" s="3"/>
-    </row>
-    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -2462,8 +2602,9 @@
       <c r="O37" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P37" s="3"/>
+    </row>
+    <row r="38" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -2492,17 +2633,20 @@
         <v>72</v>
       </c>
       <c r="J38" s="4"/>
-      <c r="K38" s="3"/>
+      <c r="K38" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="L38" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M38" s="8" t="s">
         <v>51</v>
       </c>
       <c r="N38" s="8"/>
       <c r="O38" s="3"/>
-    </row>
-    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P38" s="3"/>
+    </row>
+    <row r="39" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -2533,7 +2677,7 @@
       <c r="J39" s="4"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M39" s="8" t="s">
         <v>103</v>
@@ -2542,8 +2686,9 @@
       <c r="O39" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P39" s="3"/>
+    </row>
+    <row r="40" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -2574,9 +2719,11 @@
       <c r="J40" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K40" s="3"/>
+      <c r="K40" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="L40" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M40" s="8" t="s">
         <v>50</v>
@@ -2585,8 +2732,9 @@
       <c r="O40" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P40" s="3"/>
+    </row>
+    <row r="41" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -2621,7 +2769,7 @@
         <v>95</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M41" s="8" t="s">
         <v>51</v>
@@ -2632,8 +2780,9 @@
       <c r="O41" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P41" s="3"/>
+    </row>
+    <row r="42" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -2664,15 +2813,16 @@
       <c r="J42" s="4"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M42" s="8" t="s">
         <v>53</v>
       </c>
       <c r="N42" s="8"/>
       <c r="O42" s="3"/>
-    </row>
-    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P42" s="3"/>
+    </row>
+    <row r="43" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -2712,8 +2862,11 @@
       <c r="O43" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P43" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -2744,15 +2897,16 @@
       <c r="J44" s="4"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M44" s="8" t="s">
         <v>51</v>
       </c>
       <c r="N44" s="8"/>
       <c r="O44" s="3"/>
-    </row>
-    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P44" s="3"/>
+    </row>
+    <row r="45" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -2785,15 +2939,16 @@
       </c>
       <c r="K45" s="3"/>
       <c r="L45" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M45" s="8" t="s">
         <v>140</v>
       </c>
       <c r="N45" s="8"/>
       <c r="O45" s="3"/>
-    </row>
-    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P45" s="3"/>
+    </row>
+    <row r="46" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -2826,7 +2981,7 @@
         <v>95</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M46" s="8" t="s">
         <v>51</v>
@@ -2835,8 +2990,9 @@
         <v>143</v>
       </c>
       <c r="O46" s="3"/>
-    </row>
-    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P46" s="3"/>
+    </row>
+    <row r="47" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -2874,8 +3030,9 @@
       </c>
       <c r="N47" s="8"/>
       <c r="O47" s="3"/>
-    </row>
-    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P47" s="3"/>
+    </row>
+    <row r="48" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -2917,8 +3074,11 @@
       <c r="O48" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P48" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -2949,7 +3109,7 @@
       <c r="J49" s="4"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M49" s="8" t="s">
         <v>53</v>
@@ -2958,8 +3118,9 @@
       <c r="O49" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P49" s="3"/>
+    </row>
+    <row r="50" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -2990,7 +3151,7 @@
       <c r="J50" s="4"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M50" s="8" t="s">
         <v>103</v>
@@ -2999,8 +3160,9 @@
       <c r="O50" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P50" s="3"/>
+    </row>
+    <row r="51" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3031,15 +3193,18 @@
       <c r="J51" s="4"/>
       <c r="K51" s="3"/>
       <c r="L51" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M51" s="8" t="s">
         <v>59</v>
       </c>
       <c r="N51" s="8"/>
       <c r="O51" s="3"/>
-    </row>
-    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P51" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3070,7 +3235,7 @@
       <c r="J52" s="4"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M52" s="8" t="s">
         <v>54</v>
@@ -3079,8 +3244,9 @@
       <c r="O52" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P52" s="3"/>
+    </row>
+    <row r="53" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3122,8 +3288,11 @@
       <c r="O53" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P53" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -3146,7 +3315,7 @@
         <v>25</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>132</v>
@@ -3154,7 +3323,7 @@
       <c r="J54" s="4"/>
       <c r="K54" s="3"/>
       <c r="L54" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M54" s="8" t="s">
         <v>94</v>
@@ -3163,8 +3332,11 @@
       <c r="O54" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P54" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -3187,15 +3359,15 @@
         <v>25</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M55" s="8" t="s">
         <v>94</v>
@@ -3204,8 +3376,9 @@
       <c r="O55" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P55" s="3"/>
+    </row>
+    <row r="56" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -3231,22 +3404,23 @@
         <v>135</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>134</v>
       </c>
       <c r="K56" s="3"/>
       <c r="L56" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M56" s="8" t="s">
         <v>51</v>
       </c>
       <c r="N56" s="8"/>
       <c r="O56" s="3"/>
-    </row>
-    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P56" s="3"/>
+    </row>
+    <row r="57" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -3288,8 +3462,11 @@
       <c r="O57" s="3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P57" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -3312,7 +3489,7 @@
         <v>25</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>117</v>
@@ -3320,7 +3497,7 @@
       <c r="J58" s="4"/>
       <c r="K58" s="3"/>
       <c r="L58" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M58" s="8" t="s">
         <v>118</v>
@@ -3329,8 +3506,9 @@
       <c r="O58" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P58" s="3"/>
+    </row>
+    <row r="59" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -3353,7 +3531,7 @@
         <v>25</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>117</v>
@@ -3361,7 +3539,7 @@
       <c r="J59" s="4"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M59" s="8" t="s">
         <v>94</v>
@@ -3370,8 +3548,9 @@
       <c r="O59" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P59" s="3"/>
+    </row>
+    <row r="60" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -3394,23 +3573,28 @@
         <v>25</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="J60" s="4"/>
+        <v>144</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="K60" s="3"/>
       <c r="L60" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M60" s="8" t="s">
         <v>59</v>
       </c>
       <c r="N60" s="8"/>
       <c r="O60" s="3"/>
-    </row>
-    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P60" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -3433,15 +3617,15 @@
         <v>25</v>
       </c>
       <c r="H61" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="I61" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="I61" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="J61" s="4"/>
       <c r="K61" s="3"/>
       <c r="L61" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M61" s="8" t="s">
         <v>73</v>
@@ -3450,8 +3634,9 @@
       <c r="O61" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P61" s="3"/>
+    </row>
+    <row r="62" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -3474,15 +3659,15 @@
         <v>25</v>
       </c>
       <c r="H62" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="I62" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="J62" s="4"/>
       <c r="K62" s="3"/>
       <c r="L62" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M62" s="8" t="s">
         <v>56</v>
@@ -3491,8 +3676,9 @@
       <c r="O62" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P62" s="3"/>
+    </row>
+    <row r="63" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -3515,15 +3701,15 @@
         <v>25</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J63" s="4"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="M63" s="8" t="s">
         <v>90</v>
@@ -3532,16 +3718,17 @@
       <c r="O63" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P63" s="3"/>
+    </row>
+    <row r="64" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>63</v>
       </c>
       <c r="B64" s="3">
-        <v>1.2942899999999999</v>
+        <v>1.33355</v>
       </c>
       <c r="C64" s="3">
-        <v>103.81654899999999</v>
+        <v>103.86521999999999</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>143</v>
@@ -3555,30 +3742,37 @@
       <c r="G64" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H64" s="3"/>
+      <c r="H64" s="3" t="s">
+        <v>168</v>
+      </c>
       <c r="I64" s="3" t="s">
-        <v>117</v>
+        <v>167</v>
       </c>
       <c r="J64" s="4"/>
-      <c r="K64" s="3"/>
+      <c r="K64" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="L64" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M64" s="8"/>
+        <v>185</v>
+      </c>
+      <c r="M64" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="N64" s="8"/>
       <c r="O64" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P64" s="3"/>
+    </row>
+    <row r="65" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>64</v>
       </c>
       <c r="B65" s="3">
-        <v>1.3220970000000001</v>
+        <v>1.3472249999999999</v>
       </c>
       <c r="C65" s="3">
-        <v>103.847273</v>
+        <v>103.694941</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>143</v>
@@ -3592,18 +3786,29 @@
       <c r="G65" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
+      <c r="H65" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>170</v>
+      </c>
       <c r="J65" s="4"/>
-      <c r="K65" s="3"/>
+      <c r="K65" s="3" t="s">
+        <v>169</v>
+      </c>
       <c r="L65" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M65" s="8"/>
+        <v>185</v>
+      </c>
+      <c r="M65" s="8" t="s">
+        <v>103</v>
+      </c>
       <c r="N65" s="8"/>
       <c r="O65" s="3"/>
-    </row>
-    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P65" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -3628,27 +3833,34 @@
       <c r="H66" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="I66" s="3"/>
+      <c r="I66" s="3" t="s">
+        <v>174</v>
+      </c>
       <c r="J66" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="K66" s="3"/>
+        <v>160</v>
+      </c>
+      <c r="K66" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="L66" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M66" s="8"/>
+        <v>185</v>
+      </c>
+      <c r="M66" s="8" t="s">
+        <v>124</v>
+      </c>
       <c r="N66" s="8"/>
       <c r="O66" s="3"/>
-    </row>
-    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P66" s="3"/>
+    </row>
+    <row r="67" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>66</v>
       </c>
       <c r="B67" s="3">
-        <v>1.294427</v>
+        <v>1.353804</v>
       </c>
       <c r="C67" s="3">
-        <v>103.816418</v>
+        <v>103.86051</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>143</v>
@@ -3662,22 +3874,31 @@
       <c r="G67" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H67" s="3"/>
+      <c r="H67" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="I67" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="J67" s="4"/>
-      <c r="K67" s="3"/>
+        <v>176</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="K67" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="L67" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M67" s="8"/>
+        <v>185</v>
+      </c>
+      <c r="M67" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="N67" s="8"/>
       <c r="O67" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P67" s="3"/>
+    </row>
+    <row r="68" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -3700,29 +3921,226 @@
         <v>25</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>117</v>
+        <v>177</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="K68" s="3"/>
+        <v>152</v>
+      </c>
+      <c r="K68" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="L68" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M68" s="8"/>
+        <v>185</v>
+      </c>
+      <c r="M68" s="8" t="s">
+        <v>90</v>
+      </c>
       <c r="N68" s="8"/>
       <c r="O68" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
-    </row>
-    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
+      <c r="P68" s="3"/>
+    </row>
+    <row r="69" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <v>68</v>
+      </c>
+      <c r="B69" s="3">
+        <v>1.2942830000000001</v>
+      </c>
+      <c r="C69" s="3">
+        <v>103.81647</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E69" s="3">
+        <v>79</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M69" s="8"/>
+      <c r="N69" s="8"/>
+      <c r="O69" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="P69" s="3"/>
+    </row>
+    <row r="70" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <v>69</v>
+      </c>
+      <c r="B70" s="3">
+        <v>1.4058139999999999</v>
+      </c>
+      <c r="C70" s="3">
+        <v>103.865775</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E70" s="3">
+        <v>26</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J70" s="4"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M70" s="8"/>
+      <c r="N70" s="8"/>
+      <c r="O70" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="P70" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>70</v>
+      </c>
+      <c r="B71" s="3">
+        <v>1.294286</v>
+      </c>
+      <c r="C71" s="3">
+        <v>103.816588</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E71" s="3">
+        <v>27</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M71" s="8"/>
+      <c r="N71" s="8"/>
+      <c r="O71" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="P71" s="3"/>
+    </row>
+    <row r="72" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>71</v>
+      </c>
+      <c r="B72" s="3">
+        <v>1.2942830000000001</v>
+      </c>
+      <c r="C72" s="3">
+        <v>103.816231</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E72" s="3">
+        <v>25</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M72" s="8"/>
+      <c r="N72" s="8"/>
+      <c r="O72" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="P72" s="3"/>
+    </row>
+    <row r="73" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <v>72</v>
+      </c>
+      <c r="B73" s="3">
+        <v>1.31307</v>
+      </c>
+      <c r="C73" s="3">
+        <v>103.854325</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E73" s="3">
+        <v>40</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="M73" s="8"/>
+      <c r="N73" s="8"/>
+      <c r="O73" s="3"/>
+      <c r="P73" s="3" t="s">
+        <v>178</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update data on Feb 16
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="206">
   <si>
     <t>Male</t>
   </si>
@@ -443,9 +443,6 @@
     <t>Feb-13</t>
   </si>
   <si>
-    <t>50</t>
-  </si>
-  <si>
     <t>Mei Hwan Drive</t>
   </si>
   <si>
@@ -530,9 +527,6 @@
     <t>72</t>
   </si>
   <si>
-    <t>66</t>
-  </si>
-  <si>
     <t>66, 70</t>
   </si>
   <si>
@@ -615,6 +609,57 @@
   </si>
   <si>
     <t>National University of Singapore, Grace Assembly of God</t>
+  </si>
+  <si>
+    <t>Feb-16</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>Lorong 8 Toa Payoh</t>
+  </si>
+  <si>
+    <t>SAF serviceman</t>
+  </si>
+  <si>
+    <t>Mei Ling Street</t>
+  </si>
+  <si>
+    <t>Hi-Yew Technology Pte Ltd (3031A Ubi Road), Grace Assembly of God, Urgent Care Centre at Alexandra Hospital(AH)</t>
+  </si>
+  <si>
+    <t>AH</t>
+  </si>
+  <si>
+    <t>Grace Assembly of God, Bethany Presbyterian Church (364A Paya Lebar Road)</t>
+  </si>
+  <si>
+    <t>Grace Assembly of God, God’s Kingdom Bread of Life Church (37 Jalan Pemimpin), HipVan Singapore (19 Kallang Avenue)</t>
+  </si>
+  <si>
+    <t>God’s Kingdom Bread of Life Church, Grace Assembly of God, construction site at Fernvale Lane, GP clinic, Sengkang General Hospital</t>
+  </si>
+  <si>
+    <t>Fernvale Road</t>
+  </si>
+  <si>
+    <t>Marina Bay Sands Casino, Aim Heng Car Service Pte Ltd (Woodlands Industrial Park), GP clinic</t>
+  </si>
+  <si>
+    <t>Woodlands Crescent</t>
+  </si>
+  <si>
+    <t>Grace Assembly of God (Tanglin) (355 Tanglin Road), Building 613 of Tengah Air Base, GP Clinic</t>
+  </si>
+  <si>
+    <t>50, 65</t>
+  </si>
+  <si>
+    <t>55, 65</t>
   </si>
 </sst>
 </file>
@@ -974,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P73"/>
+  <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D33" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1045,7 +1090,7 @@
         <v>98</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -1082,7 +1127,7 @@
         <v>102</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N2" s="8"/>
       <c r="O2" s="3"/>
@@ -1124,7 +1169,7 @@
         <v>102</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>59</v>
@@ -1161,14 +1206,14 @@
         <v>3</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
         <v>102</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N4" s="8"/>
       <c r="O4" s="3"/>
@@ -1210,7 +1255,7 @@
         <v>102</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N5" s="8" t="s">
         <v>124</v>
@@ -1376,7 +1421,7 @@
         <v>102</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="3" t="s">
@@ -1418,7 +1463,7 @@
         <v>102</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="3" t="s">
@@ -1455,7 +1500,7 @@
         <v>17</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>95</v>
@@ -1464,7 +1509,7 @@
         <v>102</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N11" s="8" t="s">
         <v>90</v>
@@ -1552,7 +1597,7 @@
         <v>102</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N13" s="8" t="s">
         <v>124</v>
@@ -1675,7 +1720,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M16" s="8" t="s">
         <v>51</v>
@@ -1718,7 +1763,7 @@
         <v>102</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N17" s="8"/>
       <c r="O17" s="3"/>
@@ -1753,13 +1798,13 @@
         <v>1</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>95</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M18" s="8" t="s">
         <v>51</v>
@@ -1885,7 +1930,7 @@
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M21" s="8" t="s">
         <v>47</v>
@@ -1932,7 +1977,7 @@
         <v>105</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N22" s="8"/>
       <c r="O22" s="3" t="s">
@@ -1973,7 +2018,7 @@
         <v>95</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M23" s="8" t="s">
         <v>51</v>
@@ -2015,7 +2060,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M24" s="8" t="s">
         <v>51</v>
@@ -2059,19 +2104,19 @@
         <v>95</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M25" s="8" t="s">
         <v>51</v>
       </c>
       <c r="N25" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O25" s="3" t="s">
         <v>114</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -2103,13 +2148,13 @@
         <v>35</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>95</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M26" s="8" t="s">
         <v>46</v>
@@ -2151,7 +2196,7 @@
         <v>21</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>95</v>
@@ -2160,7 +2205,7 @@
         <v>102</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N27" s="8" t="s">
         <v>90</v>
@@ -2201,17 +2246,17 @@
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N28" s="8"/>
       <c r="O28" s="3" t="s">
         <v>114</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -2243,14 +2288,14 @@
         <v>36</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M29" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N29" s="8"/>
       <c r="O29" s="3" t="s">
@@ -2289,7 +2334,7 @@
         <v>95</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M30" s="8" t="s">
         <v>49</v>
@@ -2331,13 +2376,13 @@
         <v>95</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O31" s="3" t="s">
         <v>115</v>
@@ -2375,7 +2420,7 @@
       <c r="J32" s="4"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M32" s="8" t="s">
         <v>45</v>
@@ -2417,10 +2462,10 @@
       <c r="J33" s="4"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M33" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N33" s="8"/>
       <c r="O33" s="3"/>
@@ -2457,7 +2502,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M34" s="8" t="s">
         <v>51</v>
@@ -2503,7 +2548,7 @@
         <v>95</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M35" s="8" t="s">
         <v>48</v>
@@ -2547,7 +2592,7 @@
       <c r="J36" s="4"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M36" s="8" t="s">
         <v>52</v>
@@ -2634,10 +2679,10 @@
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M38" s="8" t="s">
         <v>51</v>
@@ -2677,7 +2722,7 @@
       <c r="J39" s="4"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M39" s="8" t="s">
         <v>103</v>
@@ -2720,15 +2765,17 @@
         <v>82</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>174</v>
+        <v>95</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M40" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="N40" s="8"/>
+      <c r="N40" s="8" t="s">
+        <v>189</v>
+      </c>
       <c r="O40" s="3" t="s">
         <v>115</v>
       </c>
@@ -2769,7 +2816,7 @@
         <v>95</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M41" s="8" t="s">
         <v>51</v>
@@ -2813,7 +2860,7 @@
       <c r="J42" s="4"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M42" s="8" t="s">
         <v>53</v>
@@ -2862,8 +2909,8 @@
       <c r="O43" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="P43" t="s">
-        <v>179</v>
+      <c r="P43" s="3" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -2897,7 +2944,7 @@
       <c r="J44" s="4"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M44" s="8" t="s">
         <v>51</v>
@@ -2939,10 +2986,10 @@
       </c>
       <c r="K45" s="3"/>
       <c r="L45" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M45" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N45" s="8"/>
       <c r="O45" s="3"/>
@@ -2981,13 +3028,13 @@
         <v>95</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M46" s="8" t="s">
         <v>51</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
@@ -3074,8 +3121,8 @@
       <c r="O48" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="P48" t="s">
-        <v>179</v>
+      <c r="P48" s="3" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -3109,7 +3156,7 @@
       <c r="J49" s="4"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M49" s="8" t="s">
         <v>53</v>
@@ -3151,7 +3198,7 @@
       <c r="J50" s="4"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M50" s="8" t="s">
         <v>103</v>
@@ -3167,10 +3214,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="3">
-        <v>1.278713</v>
+        <v>1.3539159999999999</v>
       </c>
       <c r="C51" s="3">
-        <v>103.85458199999999</v>
+        <v>103.86077299999999</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>124</v>
@@ -3185,15 +3232,17 @@
         <v>25</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I51" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="J51" s="4"/>
+      <c r="J51" s="4" t="s">
+        <v>205</v>
+      </c>
       <c r="K51" s="3"/>
       <c r="L51" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M51" s="8" t="s">
         <v>59</v>
@@ -3201,7 +3250,7 @@
       <c r="N51" s="8"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -3235,7 +3284,7 @@
       <c r="J52" s="4"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M52" s="8" t="s">
         <v>54</v>
@@ -3288,8 +3337,8 @@
       <c r="O53" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="P53" t="s">
-        <v>179</v>
+      <c r="P53" s="3" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="54" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -3315,17 +3364,17 @@
         <v>25</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J54" s="4"/>
       <c r="K54" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M54" s="8" t="s">
         <v>94</v>
@@ -3335,7 +3384,7 @@
         <v>117</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -3361,15 +3410,15 @@
         <v>25</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M55" s="8" t="s">
         <v>94</v>
@@ -3385,10 +3434,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="3">
-        <v>1.3538140000000001</v>
+        <v>1.3542670000000001</v>
       </c>
       <c r="C56" s="3">
-        <v>103.860564</v>
+        <v>103.860159</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>132</v>
@@ -3403,17 +3452,17 @@
         <v>25</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>133</v>
+        <v>204</v>
       </c>
       <c r="K56" s="3"/>
       <c r="L56" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M56" s="8" t="s">
         <v>51</v>
@@ -3464,8 +3513,8 @@
       <c r="O57" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="P57" t="s">
-        <v>179</v>
+      <c r="P57" s="3" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -3491,7 +3540,7 @@
         <v>25</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>117</v>
@@ -3499,7 +3548,7 @@
       <c r="J58" s="4"/>
       <c r="K58" s="3"/>
       <c r="L58" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M58" s="8" t="s">
         <v>118</v>
@@ -3533,7 +3582,7 @@
         <v>25</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>117</v>
@@ -3541,7 +3590,7 @@
       <c r="J59" s="4"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M59" s="8" t="s">
         <v>94</v>
@@ -3575,25 +3624,25 @@
         <v>25</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K60" s="3"/>
       <c r="L60" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M60" s="8" t="s">
         <v>59</v>
       </c>
       <c r="N60" s="8"/>
       <c r="O60" s="3"/>
-      <c r="P60" t="s">
-        <v>180</v>
+      <c r="P60" s="3" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -3619,15 +3668,15 @@
         <v>25</v>
       </c>
       <c r="H61" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="I61" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="I61" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="J61" s="4"/>
       <c r="K61" s="3"/>
       <c r="L61" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M61" s="8" t="s">
         <v>73</v>
@@ -3661,15 +3710,15 @@
         <v>25</v>
       </c>
       <c r="H62" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="I62" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="J62" s="4"/>
       <c r="K62" s="3"/>
       <c r="L62" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M62" s="8" t="s">
         <v>56</v>
@@ -3703,15 +3752,15 @@
         <v>25</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J63" s="4"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M63" s="8" t="s">
         <v>90</v>
@@ -3733,7 +3782,7 @@
         <v>103.86521999999999</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E64" s="3">
         <v>54</v>
@@ -3745,17 +3794,17 @@
         <v>25</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J64" s="4"/>
       <c r="K64" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M64" s="8" t="s">
         <v>94</v>
@@ -3777,7 +3826,7 @@
         <v>103.694941</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E65" s="3">
         <v>50</v>
@@ -3789,17 +3838,17 @@
         <v>25</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J65" s="4"/>
       <c r="K65" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M65" s="8" t="s">
         <v>103</v>
@@ -3807,7 +3856,7 @@
       <c r="N65" s="8"/>
       <c r="O65" s="3"/>
       <c r="P65" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -3821,7 +3870,7 @@
         <v>103.86065000000001</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E66" s="3">
         <v>61</v>
@@ -3833,19 +3882,19 @@
         <v>25</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M66" s="8" t="s">
         <v>124</v>
@@ -3865,7 +3914,7 @@
         <v>103.86051</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E67" s="3">
         <v>28</v>
@@ -3877,19 +3926,19 @@
         <v>25</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M67" s="8" t="s">
         <v>50</v>
@@ -3911,7 +3960,7 @@
         <v>103.703937</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E68" s="3">
         <v>56</v>
@@ -3923,19 +3972,19 @@
         <v>25</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M68" s="8" t="s">
         <v>90</v>
@@ -3951,13 +4000,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="3">
-        <v>1.2942830000000001</v>
+        <v>1.354034</v>
       </c>
       <c r="C69" s="3">
-        <v>103.81647</v>
+        <v>103.86039</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E69" s="3">
         <v>79</v>
@@ -3968,18 +4017,22 @@
       <c r="G69" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H69" s="3"/>
+      <c r="H69" s="3" t="s">
+        <v>133</v>
+      </c>
       <c r="I69" s="3" t="s">
-        <v>117</v>
+        <v>197</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K69" s="3"/>
       <c r="L69" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="M69" s="8"/>
+        <v>182</v>
+      </c>
+      <c r="M69" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="N69" s="8"/>
       <c r="O69" s="3" t="s">
         <v>117</v>
@@ -3997,7 +4050,7 @@
         <v>103.865775</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E70" s="3">
         <v>26</v>
@@ -4013,17 +4066,21 @@
         <v>116</v>
       </c>
       <c r="J70" s="4"/>
-      <c r="K70" s="3"/>
+      <c r="K70" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="L70" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="M70" s="8"/>
+      <c r="M70" s="8" t="s">
+        <v>118</v>
+      </c>
       <c r="N70" s="8"/>
       <c r="O70" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="P70" t="s">
-        <v>179</v>
+      <c r="P70" s="3" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="71" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -4031,13 +4088,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="3">
-        <v>1.294286</v>
+        <v>1.353739</v>
       </c>
       <c r="C71" s="3">
-        <v>103.816588</v>
+        <v>103.860224</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E71" s="3">
         <v>27</v>
@@ -4048,18 +4105,24 @@
       <c r="G71" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H71" s="3"/>
+      <c r="H71" s="3" t="s">
+        <v>133</v>
+      </c>
       <c r="I71" s="3" t="s">
-        <v>117</v>
+        <v>198</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="K71" s="3"/>
+        <v>162</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="L71" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="M71" s="8"/>
+        <v>182</v>
+      </c>
+      <c r="M71" s="8" t="s">
+        <v>103</v>
+      </c>
       <c r="N71" s="8"/>
       <c r="O71" s="3" t="s">
         <v>117</v>
@@ -4077,7 +4140,7 @@
         <v>103.816231</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E72" s="3">
         <v>25</v>
@@ -4088,18 +4151,24 @@
       <c r="G72" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H72" s="3"/>
+      <c r="H72" s="3" t="s">
+        <v>200</v>
+      </c>
       <c r="I72" s="3" t="s">
-        <v>117</v>
+        <v>199</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="K72" s="3"/>
+        <v>161</v>
+      </c>
+      <c r="K72" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="L72" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="M72" s="8"/>
+        <v>182</v>
+      </c>
+      <c r="M72" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="N72" s="8"/>
       <c r="O72" s="3" t="s">
         <v>117</v>
@@ -4117,7 +4186,7 @@
         <v>103.854325</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E73" s="3">
         <v>40</v>
@@ -4128,21 +4197,163 @@
       <c r="G73" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
+      <c r="H73" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>201</v>
+      </c>
       <c r="J73" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="K73" s="3"/>
+        <v>159</v>
+      </c>
+      <c r="K73" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="L73" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="M73" s="8"/>
+      <c r="M73" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="N73" s="8"/>
       <c r="O73" s="3"/>
       <c r="P73" s="3" t="s">
-        <v>177</v>
-      </c>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
+        <v>73</v>
+      </c>
+      <c r="B74" s="3">
+        <v>1.3398159999999999</v>
+      </c>
+      <c r="C74" s="3">
+        <v>103.856009</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E74" s="3">
+        <v>43</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="K74" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L74" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M74" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N74" s="8"/>
+      <c r="O74" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="P74" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <v>74</v>
+      </c>
+      <c r="B75" s="3">
+        <v>1.2943039999999999</v>
+      </c>
+      <c r="C75" s="3">
+        <v>103.803596</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E75" s="3">
+        <v>29</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="J75" s="4"/>
+      <c r="K75" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L75" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M75" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="N75" s="8"/>
+      <c r="O75" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="P75" s="3"/>
+    </row>
+    <row r="76" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>75</v>
+      </c>
+      <c r="B76" s="3">
+        <v>1.3543860000000001</v>
+      </c>
+      <c r="C76" s="3">
+        <v>103.877948</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E76" s="3">
+        <v>71</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I76" s="3"/>
+      <c r="J76" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="K76" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L76" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M76" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="N76" s="8"/>
+      <c r="O76" s="3"/>
+      <c r="P76" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update on Feb 17
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="209">
   <si>
     <t>Male</t>
   </si>
@@ -660,6 +660,15 @@
   </si>
   <si>
     <t>55, 65</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>KK</t>
+  </si>
+  <si>
+    <t>Feb-17</t>
   </si>
 </sst>
 </file>
@@ -1019,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P76"/>
+  <dimension ref="A1:P78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1678,14 +1687,18 @@
         <v>24</v>
       </c>
       <c r="J15" s="4"/>
-      <c r="K15" s="3"/>
+      <c r="K15" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L15" s="3" t="s">
         <v>102</v>
       </c>
       <c r="M15" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="N15" s="8"/>
+      <c r="N15" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
     </row>
@@ -1718,14 +1731,18 @@
         <v>1</v>
       </c>
       <c r="J16" s="4"/>
-      <c r="K16" s="3"/>
+      <c r="K16" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L16" s="3" t="s">
         <v>182</v>
       </c>
       <c r="M16" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="N16" s="8"/>
+      <c r="N16" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
     </row>
@@ -2418,14 +2435,18 @@
         <v>61</v>
       </c>
       <c r="J32" s="4"/>
-      <c r="K32" s="3"/>
+      <c r="K32" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L32" s="3" t="s">
         <v>182</v>
       </c>
       <c r="M32" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="N32" s="8"/>
+      <c r="N32" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="O32" s="3" t="s">
         <v>113</v>
       </c>
@@ -3154,14 +3175,18 @@
         <v>119</v>
       </c>
       <c r="J49" s="4"/>
-      <c r="K49" s="3"/>
+      <c r="K49" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L49" s="3" t="s">
         <v>182</v>
       </c>
       <c r="M49" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="N49" s="8"/>
+      <c r="N49" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="O49" s="3" t="s">
         <v>117</v>
       </c>
@@ -3891,7 +3916,7 @@
         <v>158</v>
       </c>
       <c r="K66" s="3" t="s">
-        <v>172</v>
+        <v>95</v>
       </c>
       <c r="L66" s="3" t="s">
         <v>182</v>
@@ -3899,7 +3924,9 @@
       <c r="M66" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="N66" s="8"/>
+      <c r="N66" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="O66" s="3"/>
       <c r="P66" s="3"/>
     </row>
@@ -4355,6 +4382,70 @@
       <c r="O76" s="3"/>
       <c r="P76" s="3"/>
     </row>
+    <row r="77" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
+        <v>76</v>
+      </c>
+      <c r="B77" s="3">
+        <v>1.310438</v>
+      </c>
+      <c r="C77">
+        <v>103.84718100000001</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E77" s="3">
+        <v>1</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K77" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="L77" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M77" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <v>77</v>
+      </c>
+      <c r="B78" s="3">
+        <v>1.3535889999999999</v>
+      </c>
+      <c r="C78">
+        <v>103.859931</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E78" s="3">
+        <v>35</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J78" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="K78" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="L78" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update on Feb-18 data
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="215">
   <si>
     <t>Male</t>
   </si>
@@ -521,9 +521,6 @@
     <t>50, 55</t>
   </si>
   <si>
-    <t>59</t>
-  </si>
-  <si>
     <t>72</t>
   </si>
   <si>
@@ -659,16 +656,37 @@
     <t>50, 65</t>
   </si>
   <si>
-    <t>55, 65</t>
-  </si>
-  <si>
     <t>50</t>
   </si>
   <si>
-    <t>KK</t>
-  </si>
-  <si>
     <t>Feb-17</t>
+  </si>
+  <si>
+    <t>59, 79</t>
+  </si>
+  <si>
+    <t>55, 65, 77</t>
+  </si>
+  <si>
+    <t>VWO-run community hospital</t>
+  </si>
+  <si>
+    <t>Dairy Farm</t>
+  </si>
+  <si>
+    <t>Malaysian</t>
+  </si>
+  <si>
+    <t>FoodXchange @ Admiralty (8A Admiralty Street)</t>
+  </si>
+  <si>
+    <t>Feb-18</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>McNair Road</t>
   </si>
 </sst>
 </file>
@@ -1028,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P78"/>
+  <dimension ref="A1:P82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1099,7 +1117,7 @@
         <v>98</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -1215,7 +1233,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
@@ -1301,14 +1319,18 @@
         <v>10</v>
       </c>
       <c r="J6" s="4"/>
-      <c r="K6" s="3"/>
+      <c r="K6" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L6" s="3" t="s">
         <v>102</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N6" s="8"/>
+      <c r="N6" s="8" t="s">
+        <v>212</v>
+      </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
     </row>
@@ -1425,14 +1447,18 @@
         <v>10</v>
       </c>
       <c r="J9" s="4"/>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L9" s="3" t="s">
         <v>102</v>
       </c>
       <c r="M9" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="N9" s="8"/>
+      <c r="N9" s="8" t="s">
+        <v>212</v>
+      </c>
       <c r="O9" s="3" t="s">
         <v>113</v>
       </c>
@@ -1509,7 +1535,7 @@
         <v>17</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>95</v>
@@ -1697,7 +1723,7 @@
         <v>49</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
@@ -1735,13 +1761,13 @@
         <v>95</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M16" s="8" t="s">
         <v>51</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
@@ -1815,13 +1841,13 @@
         <v>1</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>95</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M18" s="8" t="s">
         <v>51</v>
@@ -1947,7 +1973,7 @@
       </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M21" s="8" t="s">
         <v>47</v>
@@ -1989,14 +2015,18 @@
       <c r="J22" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="K22" s="3"/>
+      <c r="K22" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L22" s="3" t="s">
         <v>105</v>
       </c>
       <c r="M22" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="N22" s="8"/>
+      <c r="N22" s="8" t="s">
+        <v>212</v>
+      </c>
       <c r="O22" s="3" t="s">
         <v>114</v>
       </c>
@@ -2035,7 +2065,7 @@
         <v>95</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M23" s="8" t="s">
         <v>51</v>
@@ -2077,7 +2107,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M24" s="8" t="s">
         <v>51</v>
@@ -2121,7 +2151,7 @@
         <v>95</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M25" s="8" t="s">
         <v>51</v>
@@ -2133,7 +2163,7 @@
         <v>114</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -2165,13 +2195,13 @@
         <v>35</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>95</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M26" s="8" t="s">
         <v>46</v>
@@ -2213,7 +2243,7 @@
         <v>21</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>95</v>
@@ -2263,7 +2293,7 @@
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M28" s="8" t="s">
         <v>138</v>
@@ -2273,7 +2303,7 @@
         <v>114</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -2309,7 +2339,7 @@
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M29" s="8" t="s">
         <v>138</v>
@@ -2351,7 +2381,7 @@
         <v>95</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M30" s="8" t="s">
         <v>49</v>
@@ -2393,7 +2423,7 @@
         <v>95</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M31" s="8" t="s">
         <v>139</v>
@@ -2439,13 +2469,13 @@
         <v>95</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M32" s="8" t="s">
         <v>45</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="O32" s="3" t="s">
         <v>113</v>
@@ -2483,7 +2513,7 @@
       <c r="J33" s="4"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M33" s="8" t="s">
         <v>138</v>
@@ -2523,7 +2553,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M34" s="8" t="s">
         <v>51</v>
@@ -2569,7 +2599,7 @@
         <v>95</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M35" s="8" t="s">
         <v>48</v>
@@ -2613,7 +2643,7 @@
       <c r="J36" s="4"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M36" s="8" t="s">
         <v>52</v>
@@ -2700,10 +2730,10 @@
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M38" s="8" t="s">
         <v>51</v>
@@ -2741,14 +2771,18 @@
         <v>74</v>
       </c>
       <c r="J39" s="4"/>
-      <c r="K39" s="3"/>
+      <c r="K39" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L39" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M39" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="N39" s="8"/>
+      <c r="N39" s="8" t="s">
+        <v>212</v>
+      </c>
       <c r="O39" s="3" t="s">
         <v>113</v>
       </c>
@@ -2789,13 +2823,13 @@
         <v>95</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M40" s="8" t="s">
         <v>50</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O40" s="3" t="s">
         <v>115</v>
@@ -2837,7 +2871,7 @@
         <v>95</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M41" s="8" t="s">
         <v>51</v>
@@ -2881,7 +2915,7 @@
       <c r="J42" s="4"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M42" s="8" t="s">
         <v>53</v>
@@ -2931,7 +2965,7 @@
         <v>116</v>
       </c>
       <c r="P43" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -2965,7 +2999,7 @@
       <c r="J44" s="4"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M44" s="8" t="s">
         <v>51</v>
@@ -3007,7 +3041,7 @@
       </c>
       <c r="K45" s="3"/>
       <c r="L45" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M45" s="8" t="s">
         <v>138</v>
@@ -3049,7 +3083,7 @@
         <v>95</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M46" s="8" t="s">
         <v>51</v>
@@ -3143,7 +3177,7 @@
         <v>116</v>
       </c>
       <c r="P48" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -3179,13 +3213,13 @@
         <v>95</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M49" s="8" t="s">
         <v>53</v>
       </c>
       <c r="N49" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="O49" s="3" t="s">
         <v>117</v>
@@ -3223,7 +3257,7 @@
       <c r="J50" s="4"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M50" s="8" t="s">
         <v>103</v>
@@ -3263,11 +3297,11 @@
         <v>123</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K51" s="3"/>
       <c r="L51" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M51" s="8" t="s">
         <v>59</v>
@@ -3275,7 +3309,7 @@
       <c r="N51" s="8"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -3309,7 +3343,7 @@
       <c r="J52" s="4"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M52" s="8" t="s">
         <v>54</v>
@@ -3363,7 +3397,7 @@
         <v>116</v>
       </c>
       <c r="P53" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -3392,14 +3426,14 @@
         <v>156</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J54" s="4"/>
       <c r="K54" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M54" s="8" t="s">
         <v>94</v>
@@ -3409,7 +3443,7 @@
         <v>117</v>
       </c>
       <c r="P54" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -3443,7 +3477,7 @@
       <c r="J55" s="4"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M55" s="8" t="s">
         <v>94</v>
@@ -3483,11 +3517,11 @@
         <v>153</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K56" s="3"/>
       <c r="L56" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M56" s="8" t="s">
         <v>51</v>
@@ -3539,7 +3573,7 @@
         <v>116</v>
       </c>
       <c r="P57" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -3573,7 +3607,7 @@
       <c r="J58" s="4"/>
       <c r="K58" s="3"/>
       <c r="L58" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M58" s="8" t="s">
         <v>118</v>
@@ -3615,7 +3649,7 @@
       <c r="J59" s="4"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M59" s="8" t="s">
         <v>94</v>
@@ -3655,11 +3689,11 @@
         <v>142</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K60" s="3"/>
       <c r="L60" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M60" s="8" t="s">
         <v>59</v>
@@ -3667,7 +3701,7 @@
       <c r="N60" s="8"/>
       <c r="O60" s="3"/>
       <c r="P60" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -3701,7 +3735,7 @@
       <c r="J61" s="4"/>
       <c r="K61" s="3"/>
       <c r="L61" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M61" s="8" t="s">
         <v>73</v>
@@ -3743,7 +3777,7 @@
       <c r="J62" s="4"/>
       <c r="K62" s="3"/>
       <c r="L62" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M62" s="8" t="s">
         <v>56</v>
@@ -3785,7 +3819,7 @@
       <c r="J63" s="4"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M63" s="8" t="s">
         <v>90</v>
@@ -3819,17 +3853,17 @@
         <v>25</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J64" s="4"/>
       <c r="K64" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M64" s="8" t="s">
         <v>94</v>
@@ -3863,17 +3897,17 @@
         <v>25</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J65" s="4"/>
       <c r="K65" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M65" s="8" t="s">
         <v>103</v>
@@ -3881,7 +3915,7 @@
       <c r="N65" s="8"/>
       <c r="O65" s="3"/>
       <c r="P65" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -3910,7 +3944,7 @@
         <v>133</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J66" s="4" t="s">
         <v>158</v>
@@ -3919,13 +3953,13 @@
         <v>95</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M66" s="8" t="s">
         <v>124</v>
       </c>
       <c r="N66" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="O66" s="3"/>
       <c r="P66" s="3"/>
@@ -3956,16 +3990,16 @@
         <v>133</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K67" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M67" s="8" t="s">
         <v>50</v>
@@ -4002,16 +4036,16 @@
         <v>146</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>150</v>
       </c>
       <c r="K68" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M68" s="8" t="s">
         <v>90</v>
@@ -4048,14 +4082,14 @@
         <v>133</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K69" s="3"/>
       <c r="L69" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M69" s="8" t="s">
         <v>51</v>
@@ -4094,7 +4128,7 @@
       </c>
       <c r="J70" s="4"/>
       <c r="K70" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L70" s="3" t="s">
         <v>104</v>
@@ -4107,7 +4141,7 @@
         <v>116</v>
       </c>
       <c r="P70" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -4136,16 +4170,16 @@
         <v>133</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K71" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L71" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M71" s="8" t="s">
         <v>103</v>
@@ -4179,19 +4213,19 @@
         <v>25</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K72" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L72" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M72" s="8" t="s">
         <v>53</v>
@@ -4225,16 +4259,16 @@
         <v>25</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="K73" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L73" s="3" t="s">
         <v>102</v>
@@ -4245,7 +4279,7 @@
       <c r="N73" s="8"/>
       <c r="O73" s="3"/>
       <c r="P73" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="74" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -4271,19 +4305,19 @@
         <v>25</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K74" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L74" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M74" s="8" t="s">
         <v>90</v>
@@ -4293,7 +4327,7 @@
         <v>117</v>
       </c>
       <c r="P74" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="75" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -4319,17 +4353,17 @@
         <v>25</v>
       </c>
       <c r="H75" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="I75" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="I75" s="3" t="s">
-        <v>195</v>
       </c>
       <c r="J75" s="4"/>
       <c r="K75" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L75" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M75" s="8" t="s">
         <v>124</v>
@@ -4351,7 +4385,7 @@
         <v>103.877948</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E76" s="3">
         <v>71</v>
@@ -4367,13 +4401,13 @@
       </c>
       <c r="I76" s="3"/>
       <c r="J76" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K76" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L76" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M76" s="8" t="s">
         <v>59</v>
@@ -4393,7 +4427,7 @@
         <v>103.84718100000001</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E77" s="3">
         <v>1</v>
@@ -4405,13 +4439,16 @@
         <v>1</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>207</v>
+        <v>95</v>
       </c>
       <c r="L77" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M77" s="10" t="s">
         <v>90</v>
+      </c>
+      <c r="N77" s="10" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="1:16" ht="21" x14ac:dyDescent="0.25">
@@ -4419,13 +4456,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="3">
-        <v>1.3535889999999999</v>
+        <v>1.320789</v>
       </c>
       <c r="C78">
-        <v>103.859931</v>
+        <v>103.859112</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E78" s="3">
         <v>35</v>
@@ -4436,14 +4473,175 @@
       <c r="G78" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="H78" t="s">
+        <v>214</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="J78" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K78" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L78" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
+      </c>
+      <c r="M78" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <v>78</v>
+      </c>
+      <c r="B79" s="3">
+        <v>1.3653550000000001</v>
+      </c>
+      <c r="C79">
+        <v>103.774413</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E79" s="3">
+        <v>57</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H79" t="s">
+        <v>209</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="K79" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L79" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M79" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="O79" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A80" s="3">
+        <v>79</v>
+      </c>
+      <c r="B80" s="3">
+        <v>1.4466920000000001</v>
+      </c>
+      <c r="C80">
+        <v>103.803037</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E80" s="3">
+        <v>35</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H80" t="s">
+        <v>201</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="K80" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L80" t="s">
+        <v>210</v>
+      </c>
+      <c r="M80" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A81" s="3">
+        <v>80</v>
+      </c>
+      <c r="B81" s="3">
+        <v>1.2934600000000001</v>
+      </c>
+      <c r="C81">
+        <v>103.783433</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E81" s="3">
+        <v>38</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="J81" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="K81" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="L81" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="O81" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
+        <v>81</v>
+      </c>
+      <c r="B82" s="3">
+        <v>1.294227</v>
+      </c>
+      <c r="C82">
+        <v>103.816554</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E82" s="3">
+        <v>50</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K82" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L82" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="O82" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data on Feb-19
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="224">
   <si>
     <t>Male</t>
   </si>
@@ -687,6 +687,33 @@
   </si>
   <si>
     <t>McNair Road</t>
+  </si>
+  <si>
+    <t>Feb-19</t>
+  </si>
+  <si>
+    <t>NTFGH</t>
+  </si>
+  <si>
+    <t>Jurong Polyclinic, GP Clinic, NTFGH emergency department</t>
+  </si>
+  <si>
+    <t>Jurong West Street 41</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>NUH, GP Clinic</t>
+  </si>
+  <si>
+    <t>NUH administration</t>
+  </si>
+  <si>
+    <t>Fernvale Link</t>
+  </si>
+  <si>
+    <t>Lower Delta Road</t>
   </si>
 </sst>
 </file>
@@ -1046,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P82"/>
+  <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1149,14 +1176,18 @@
         <v>3</v>
       </c>
       <c r="J2" s="4"/>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L2" s="3" t="s">
         <v>102</v>
       </c>
       <c r="M2" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="N2" s="8"/>
+      <c r="N2" s="8" t="s">
+        <v>215</v>
+      </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
     </row>
@@ -2511,14 +2542,18 @@
         <v>65</v>
       </c>
       <c r="J33" s="4"/>
-      <c r="K33" s="3"/>
+      <c r="K33" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L33" s="3" t="s">
         <v>181</v>
       </c>
       <c r="M33" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="N33" s="8"/>
+      <c r="N33" s="8" t="s">
+        <v>215</v>
+      </c>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
     </row>
@@ -2551,14 +2586,18 @@
         <v>63</v>
       </c>
       <c r="J34" s="4"/>
-      <c r="K34" s="3"/>
+      <c r="K34" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L34" s="3" t="s">
         <v>181</v>
       </c>
       <c r="M34" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="N34" s="8"/>
+      <c r="N34" s="8" t="s">
+        <v>215</v>
+      </c>
       <c r="O34" s="3" t="s">
         <v>113</v>
       </c>
@@ -3039,14 +3078,18 @@
       <c r="J45" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="K45" s="3"/>
+      <c r="K45" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L45" s="3" t="s">
         <v>181</v>
       </c>
       <c r="M45" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="N45" s="8"/>
+      <c r="N45" s="8" t="s">
+        <v>215</v>
+      </c>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
     </row>
@@ -3519,14 +3562,18 @@
       <c r="J56" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="K56" s="3"/>
+      <c r="K56" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="L56" s="3" t="s">
         <v>181</v>
       </c>
       <c r="M56" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="N56" s="8"/>
+      <c r="N56" s="8" t="s">
+        <v>215</v>
+      </c>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
     </row>
@@ -4574,15 +4621,15 @@
         <v>124</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>80</v>
       </c>
       <c r="B81" s="3">
-        <v>1.2934600000000001</v>
+        <v>1.3965160000000001</v>
       </c>
       <c r="C81">
-        <v>103.783433</v>
+        <v>103.87891999999999</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>212</v>
@@ -4596,8 +4643,11 @@
       <c r="G81" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="H81" t="s">
+        <v>222</v>
+      </c>
       <c r="I81" s="3" t="s">
-        <v>165</v>
+        <v>220</v>
       </c>
       <c r="J81" s="5" t="s">
         <v>213</v>
@@ -4608,19 +4658,25 @@
       <c r="L81" s="3" t="s">
         <v>181</v>
       </c>
+      <c r="M81" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="O81" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="P81" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
       <c r="B82" s="3">
-        <v>1.294227</v>
+        <v>1.280619</v>
       </c>
       <c r="C82">
-        <v>103.816554</v>
+        <v>103.82365299999999</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>212</v>
@@ -4634,13 +4690,127 @@
       <c r="G82" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="H82" t="s">
+        <v>223</v>
+      </c>
       <c r="K82" s="3" t="s">
         <v>171</v>
       </c>
       <c r="L82" s="3" t="s">
         <v>181</v>
       </c>
+      <c r="M82" s="10" t="s">
+        <v>188</v>
+      </c>
       <c r="O82" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
+        <v>82</v>
+      </c>
+      <c r="B83" s="3">
+        <v>1.348231</v>
+      </c>
+      <c r="C83">
+        <v>103.72327</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E83" s="3">
+        <v>57</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H83" t="s">
+        <v>218</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="K83" t="s">
+        <v>216</v>
+      </c>
+      <c r="L83" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M83" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
+        <v>83</v>
+      </c>
+      <c r="B84" s="3">
+        <v>1.322101</v>
+      </c>
+      <c r="C84">
+        <v>103.847257</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E84" s="3">
+        <v>54</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="K84" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L84" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="O84" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
+        <v>84</v>
+      </c>
+      <c r="B85" s="3">
+        <v>1.3221160000000001</v>
+      </c>
+      <c r="C85">
+        <v>103.847244</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E85" s="3">
+        <v>35</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J85" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="K85" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L85" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="O85" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update data on Feb-20
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="237">
   <si>
     <t>Male</t>
   </si>
@@ -677,9 +677,6 @@
     <t>Jurong West Street 41</t>
   </si>
   <si>
-    <t>Malaysia</t>
-  </si>
-  <si>
     <t>NUH, GP Clinic</t>
   </si>
   <si>
@@ -695,9 +692,6 @@
     <t>SGH</t>
   </si>
   <si>
-    <t>CGH</t>
-  </si>
-  <si>
     <t>KKH</t>
   </si>
   <si>
@@ -726,6 +720,39 @@
   </si>
   <si>
     <t>Malaysia, Plaza Singapura, Star Vista, Fusionopolis, Grace Assembly of God (Tanglin), Grace Assembly of God (Bukit Batok), GP clinics</t>
+  </si>
+  <si>
+    <t>Feb-20</t>
+  </si>
+  <si>
+    <t>Malaysia, Philemon Singapore Pte Ltd (16 Kallang Place), GP clinic</t>
+  </si>
+  <si>
+    <t>Rivervale Drive</t>
+  </si>
+  <si>
+    <t>Lonza Biologics (35 Tuas South Avenue 6), Bugis Junction, GP clinic</t>
+  </si>
+  <si>
+    <t>Aljunied Road</t>
+  </si>
+  <si>
+    <t>Sales Person</t>
+  </si>
+  <si>
+    <t>Maid</t>
+  </si>
+  <si>
+    <t>Security Officer</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Jewellry Clerk</t>
+  </si>
+  <si>
+    <t>Hospital administration</t>
   </si>
 </sst>
 </file>
@@ -1072,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1261,7 +1288,7 @@
         <v>174</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>97</v>
@@ -1381,13 +1408,16 @@
         <v>12</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>217</v>
+        <v>90</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>97</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>47</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1794,13 +1824,16 @@
         <v>3</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>216</v>
+        <v>90</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>97</v>
       </c>
       <c r="M17" s="6" t="s">
         <v>127</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1914,7 +1947,7 @@
         <v>29</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>106</v>
@@ -1924,6 +1957,9 @@
       </c>
       <c r="O20" s="2" t="s">
         <v>108</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -1969,6 +2005,9 @@
       <c r="O21" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="P21" s="2" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -2016,6 +2055,9 @@
       <c r="O22" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="P22" s="2" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -2192,6 +2234,9 @@
       <c r="O26" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="P26" s="2" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -2316,7 +2361,7 @@
         <v>132</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>173</v>
@@ -2389,10 +2434,10 @@
         <v>25</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>90</v>
@@ -2494,6 +2539,9 @@
       <c r="N33" s="6" t="s">
         <v>207</v>
       </c>
+      <c r="P33" s="2" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
@@ -2565,7 +2613,7 @@
         <v>65</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>76</v>
@@ -2584,6 +2632,9 @@
       </c>
       <c r="O35" s="2" t="s">
         <v>108</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -2615,13 +2666,16 @@
         <v>67</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>173</v>
       </c>
       <c r="M36" s="6" t="s">
         <v>52</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -2650,7 +2704,7 @@
         <v>68</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>77</v>
@@ -2697,7 +2751,7 @@
         <v>69</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>163</v>
@@ -2707,6 +2761,9 @@
       </c>
       <c r="M38" s="6" t="s">
         <v>51</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -2779,7 +2836,7 @@
         <v>73</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J40" s="3" t="s">
         <v>77</v>
@@ -2958,7 +3015,7 @@
         <v>83</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="L44" s="2" t="s">
         <v>173</v>
@@ -3010,6 +3067,9 @@
       <c r="N45" s="6" t="s">
         <v>207</v>
       </c>
+      <c r="P45" s="2" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
@@ -3078,7 +3138,7 @@
         <v>102</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>163</v>
@@ -3163,7 +3223,7 @@
         <v>113</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>90</v>
@@ -3767,7 +3827,7 @@
         <v>140</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L63" s="2" t="s">
         <v>173</v>
@@ -3937,13 +3997,16 @@
         <v>154</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="L67" s="2" t="s">
         <v>173</v>
       </c>
       <c r="M67" s="6" t="s">
         <v>50</v>
+      </c>
+      <c r="N67" s="6" t="s">
+        <v>226</v>
       </c>
       <c r="O67" s="2" t="s">
         <v>111</v>
@@ -4452,6 +4515,9 @@
       <c r="O79" s="2" t="s">
         <v>111</v>
       </c>
+      <c r="P79" s="2" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
@@ -4517,10 +4583,10 @@
         <v>25</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J81" s="3" t="s">
         <v>205</v>
@@ -4538,7 +4604,7 @@
         <v>111</v>
       </c>
       <c r="P81" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
@@ -4564,7 +4630,7 @@
         <v>25</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K82" s="2" t="s">
         <v>163</v>
@@ -4622,10 +4688,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="2">
-        <v>1.322101</v>
+        <v>1.387508</v>
       </c>
       <c r="C84" s="2">
-        <v>103.847257</v>
+        <v>103.90475499999999</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>207</v>
@@ -4639,14 +4705,20 @@
       <c r="G84" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="H84" s="2" t="s">
+        <v>228</v>
+      </c>
       <c r="I84" s="2" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="K84" s="2" t="s">
         <v>163</v>
       </c>
       <c r="L84" s="2" t="s">
         <v>173</v>
+      </c>
+      <c r="M84" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="O84" s="2" t="s">
         <v>107</v>
@@ -4657,10 +4729,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="2">
-        <v>1.3221160000000001</v>
+        <v>1.3230109999999999</v>
       </c>
       <c r="C85" s="2">
-        <v>103.847244</v>
+        <v>103.881266</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>207</v>
@@ -4674,6 +4746,12 @@
       <c r="G85" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="H85" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>229</v>
+      </c>
       <c r="J85" s="3" t="s">
         <v>205</v>
       </c>
@@ -4683,8 +4761,43 @@
       <c r="L85" s="2" t="s">
         <v>173</v>
       </c>
+      <c r="M85" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="O85" s="2" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>85</v>
+      </c>
+      <c r="B86" s="2">
+        <v>1.322109</v>
+      </c>
+      <c r="C86" s="2">
+        <v>103.847272</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E86" s="2">
+        <v>36</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="P86" s="2" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data on Feb-22
</commit_message>
<xml_diff>
--- a/rawdata.xlsx
+++ b/rawdata.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="246">
   <si>
     <t>Male</t>
   </si>
@@ -440,9 +440,6 @@
     <t>Feb-02</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>Feb-14</t>
   </si>
   <si>
@@ -692,9 +689,6 @@
     <t>SGH</t>
   </si>
   <si>
-    <t>KKH</t>
-  </si>
-  <si>
     <t>SKH</t>
   </si>
   <si>
@@ -753,6 +747,39 @@
   </si>
   <si>
     <t>Hospital administration</t>
+  </si>
+  <si>
+    <t>Feb-21</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>GP Clinics</t>
+  </si>
+  <si>
+    <t>Bukit Batok East Avenue 5</t>
+  </si>
+  <si>
+    <t>SIT student</t>
+  </si>
+  <si>
+    <t>GP Clinics, Yishun Polyclinic</t>
+  </si>
+  <si>
+    <t>Woodlands Avenue 6</t>
+  </si>
+  <si>
+    <t>Feb-22</t>
+  </si>
+  <si>
+    <t>19, 27</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>Hougang Street 91</t>
   </si>
 </sst>
 </file>
@@ -1099,10 +1126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P86"/>
+  <dimension ref="A1:P90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+      <selection activeCell="I89" sqref="I89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1198,7 @@
         <v>93</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1212,7 +1239,7 @@
         <v>127</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1285,16 +1312,19 @@
         <v>3</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>215</v>
+        <v>90</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>97</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>127</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1376,7 +1406,7 @@
         <v>46</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1417,7 +1447,7 @@
         <v>47</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1499,7 +1529,7 @@
         <v>129</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>107</v>
@@ -1534,7 +1564,7 @@
         <v>10</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>97</v>
@@ -1575,7 +1605,7 @@
         <v>17</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>90</v>
@@ -1751,7 +1781,7 @@
         <v>49</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1786,13 +1816,13 @@
         <v>90</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>51</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1833,7 +1863,7 @@
         <v>127</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1865,13 +1895,13 @@
         <v>1</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>90</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>51</v>
@@ -1909,7 +1939,7 @@
         <v>27</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>97</v>
@@ -1947,7 +1977,7 @@
         <v>29</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>215</v>
+        <v>90</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>106</v>
@@ -1955,11 +1985,14 @@
       <c r="M20" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="N20" s="6" t="s">
+        <v>242</v>
+      </c>
       <c r="O20" s="2" t="s">
         <v>108</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -1994,10 +2027,10 @@
         <v>76</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M21" s="6" t="s">
         <v>47</v>
@@ -2006,7 +2039,7 @@
         <v>108</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2050,13 +2083,13 @@
         <v>131</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O22" s="2" t="s">
         <v>108</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -2091,7 +2124,7 @@
         <v>90</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M23" s="6" t="s">
         <v>51</v>
@@ -2129,13 +2162,16 @@
         <v>1</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M24" s="6" t="s">
         <v>51</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -2173,19 +2209,19 @@
         <v>90</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M25" s="6" t="s">
         <v>51</v>
       </c>
       <c r="N25" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O25" s="2" t="s">
         <v>108</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -2217,13 +2253,13 @@
         <v>35</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>90</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M26" s="6" t="s">
         <v>46</v>
@@ -2235,7 +2271,7 @@
         <v>108</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -2267,7 +2303,7 @@
         <v>21</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>90</v>
@@ -2314,19 +2350,22 @@
         <v>76</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M28" s="6" t="s">
         <v>131</v>
       </c>
+      <c r="N28" s="6" t="s">
+        <v>235</v>
+      </c>
       <c r="O28" s="2" t="s">
         <v>108</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -2358,16 +2397,19 @@
         <v>36</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>132</v>
+        <v>243</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>216</v>
+        <v>90</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M29" s="6" t="s">
         <v>131</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>242</v>
       </c>
       <c r="O29" s="2" t="s">
         <v>108</v>
@@ -2402,7 +2444,7 @@
         <v>90</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M30" s="6" t="s">
         <v>49</v>
@@ -2434,22 +2476,22 @@
         <v>25</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>90</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M31" s="6" t="s">
         <v>128</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O31" s="2" t="s">
         <v>109</v>
@@ -2487,13 +2529,13 @@
         <v>90</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M32" s="6" t="s">
         <v>45</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O32" s="2" t="s">
         <v>107</v>
@@ -2531,16 +2573,16 @@
         <v>90</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M33" s="6" t="s">
         <v>131</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -2575,13 +2617,13 @@
         <v>90</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M34" s="6" t="s">
         <v>51</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O34" s="2" t="s">
         <v>107</v>
@@ -2613,7 +2655,7 @@
         <v>65</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>76</v>
@@ -2622,7 +2664,7 @@
         <v>90</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M35" s="6" t="s">
         <v>48</v>
@@ -2634,7 +2676,7 @@
         <v>108</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -2666,16 +2708,16 @@
         <v>67</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M36" s="6" t="s">
         <v>52</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -2704,7 +2746,7 @@
         <v>68</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>77</v>
@@ -2751,19 +2793,19 @@
         <v>69</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M38" s="6" t="s">
         <v>51</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
@@ -2798,13 +2840,13 @@
         <v>90</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M39" s="6" t="s">
         <v>98</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="O39" s="2" t="s">
         <v>107</v>
@@ -2836,7 +2878,7 @@
         <v>73</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J40" s="3" t="s">
         <v>77</v>
@@ -2845,13 +2887,13 @@
         <v>90</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M40" s="6" t="s">
         <v>50</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O40" s="2" t="s">
         <v>109</v>
@@ -2892,7 +2934,7 @@
         <v>90</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M41" s="6" t="s">
         <v>51</v>
@@ -2933,10 +2975,10 @@
         <v>79</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>53</v>
@@ -2971,7 +3013,7 @@
         <v>81</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L43" s="2" t="s">
         <v>99</v>
@@ -2983,7 +3025,7 @@
         <v>110</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -3015,10 +3057,10 @@
         <v>83</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M44" s="6" t="s">
         <v>51</v>
@@ -3059,16 +3101,16 @@
         <v>90</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M45" s="6" t="s">
         <v>131</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -3103,13 +3145,13 @@
         <v>90</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M46" s="6" t="s">
         <v>51</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -3138,10 +3180,10 @@
         <v>102</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L47" s="2" t="s">
         <v>101</v>
@@ -3182,7 +3224,7 @@
         <v>103</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L48" s="2" t="s">
         <v>99</v>
@@ -3194,7 +3236,7 @@
         <v>110</v>
       </c>
       <c r="P48" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -3223,19 +3265,19 @@
         <v>113</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>90</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M49" s="6" t="s">
         <v>53</v>
       </c>
       <c r="N49" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O49" s="2" t="s">
         <v>111</v>
@@ -3270,10 +3312,10 @@
         <v>114</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M50" s="6" t="s">
         <v>98</v>
@@ -3311,19 +3353,22 @@
         <v>116</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M51" s="6" t="s">
         <v>58</v>
       </c>
+      <c r="N51" s="6" t="s">
+        <v>235</v>
+      </c>
       <c r="P51" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -3355,13 +3400,16 @@
         <v>120</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M52" s="6" t="s">
         <v>54</v>
+      </c>
+      <c r="N52" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="O52" s="2" t="s">
         <v>111</v>
@@ -3399,7 +3447,7 @@
         <v>122</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L53" s="2" t="s">
         <v>99</v>
@@ -3411,7 +3459,7 @@
         <v>110</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -3437,16 +3485,16 @@
         <v>25</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L54" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M54" s="6" t="s">
         <v>89</v>
@@ -3455,7 +3503,7 @@
         <v>111</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -3481,16 +3529,16 @@
         <v>25</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M55" s="6" t="s">
         <v>89</v>
@@ -3525,22 +3573,22 @@
         <v>126</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>90</v>
       </c>
       <c r="L56" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M56" s="6" t="s">
         <v>51</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -3575,7 +3623,7 @@
         <v>122</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L57" s="2" t="s">
         <v>99</v>
@@ -3587,7 +3635,7 @@
         <v>110</v>
       </c>
       <c r="P57" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -3613,19 +3661,22 @@
         <v>25</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>111</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="L58" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M58" s="6" t="s">
         <v>112</v>
+      </c>
+      <c r="N58" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="O58" s="2" t="s">
         <v>111</v>
@@ -3654,16 +3705,16 @@
         <v>25</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>111</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M59" s="6" t="s">
         <v>89</v>
@@ -3695,25 +3746,25 @@
         <v>25</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M60" s="6" t="s">
         <v>58</v>
       </c>
       <c r="P60" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
@@ -3739,16 +3790,16 @@
         <v>25</v>
       </c>
       <c r="H61" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I61" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="I61" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="K61" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M61" s="6" t="s">
         <v>70</v>
@@ -3780,16 +3831,16 @@
         <v>25</v>
       </c>
       <c r="H62" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I62" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="I62" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="K62" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M62" s="6" t="s">
         <v>56</v>
@@ -3821,16 +3872,16 @@
         <v>25</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L63" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M63" s="6" t="s">
         <v>85</v>
@@ -3850,7 +3901,7 @@
         <v>103.86521999999999</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E64" s="2">
         <v>54</v>
@@ -3862,19 +3913,22 @@
         <v>25</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="L64" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M64" s="6" t="s">
         <v>89</v>
+      </c>
+      <c r="N64" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="O64" s="2" t="s">
         <v>111</v>
@@ -3891,7 +3945,7 @@
         <v>103.694941</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E65" s="2">
         <v>50</v>
@@ -3903,22 +3957,22 @@
         <v>25</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L65" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M65" s="6" t="s">
         <v>98</v>
       </c>
       <c r="P65" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
@@ -3932,7 +3986,7 @@
         <v>103.86065000000001</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E66" s="2">
         <v>61</v>
@@ -3947,22 +4001,22 @@
         <v>126</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K66" s="2" t="s">
         <v>90</v>
       </c>
       <c r="L66" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M66" s="6" t="s">
         <v>117</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
@@ -3976,7 +4030,7 @@
         <v>103.86051</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E67" s="2">
         <v>28</v>
@@ -3991,22 +4045,22 @@
         <v>126</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K67" s="2" t="s">
         <v>90</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M67" s="6" t="s">
         <v>50</v>
       </c>
       <c r="N67" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O67" s="2" t="s">
         <v>111</v>
@@ -4023,7 +4077,7 @@
         <v>103.703937</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E68" s="2">
         <v>56</v>
@@ -4035,19 +4089,19 @@
         <v>25</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L68" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M68" s="6" t="s">
         <v>85</v>
@@ -4067,7 +4121,7 @@
         <v>103.86039</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E69" s="2">
         <v>79</v>
@@ -4082,16 +4136,16 @@
         <v>126</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L69" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M69" s="6" t="s">
         <v>51</v>
@@ -4111,7 +4165,7 @@
         <v>103.865775</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E70" s="2">
         <v>26</v>
@@ -4126,7 +4180,7 @@
         <v>110</v>
       </c>
       <c r="K70" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L70" s="2" t="s">
         <v>99</v>
@@ -4138,7 +4192,7 @@
         <v>110</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
@@ -4152,7 +4206,7 @@
         <v>103.860224</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E71" s="2">
         <v>27</v>
@@ -4167,19 +4221,22 @@
         <v>126</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="L71" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M71" s="6" t="s">
         <v>98</v>
+      </c>
+      <c r="N71" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="O71" s="2" t="s">
         <v>111</v>
@@ -4196,7 +4253,7 @@
         <v>103.876135</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E72" s="2">
         <v>25</v>
@@ -4208,19 +4265,19 @@
         <v>25</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I72" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K72" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L72" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M72" s="6" t="s">
         <v>53</v>
@@ -4240,7 +4297,7 @@
         <v>103.803112</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E73" s="2">
         <v>40</v>
@@ -4252,16 +4309,16 @@
         <v>25</v>
       </c>
       <c r="H73" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K73" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L73" s="2" t="s">
         <v>97</v>
@@ -4270,7 +4327,7 @@
         <v>89</v>
       </c>
       <c r="P73" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
@@ -4284,7 +4341,7 @@
         <v>103.856009</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E74" s="2">
         <v>43</v>
@@ -4296,19 +4353,19 @@
         <v>25</v>
       </c>
       <c r="H74" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K74" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L74" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M74" s="6" t="s">
         <v>85</v>
@@ -4317,7 +4374,7 @@
         <v>111</v>
       </c>
       <c r="P74" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -4331,7 +4388,7 @@
         <v>103.803596</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E75" s="2">
         <v>29</v>
@@ -4343,16 +4400,16 @@
         <v>25</v>
       </c>
       <c r="H75" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I75" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="I75" s="2" t="s">
+      <c r="K75" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="K75" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="L75" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M75" s="6" t="s">
         <v>117</v>
@@ -4372,7 +4429,7 @@
         <v>103.877948</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E76" s="2">
         <v>71</v>
@@ -4387,13 +4444,13 @@
         <v>80</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K76" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L76" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M76" s="6" t="s">
         <v>58</v>
@@ -4410,7 +4467,7 @@
         <v>103.84718100000001</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E77" s="2">
         <v>1</v>
@@ -4425,13 +4482,13 @@
         <v>90</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M77" s="6" t="s">
         <v>85</v>
       </c>
       <c r="N77" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
@@ -4445,7 +4502,7 @@
         <v>103.859112</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E78" s="2">
         <v>35</v>
@@ -4457,19 +4514,19 @@
         <v>25</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I78" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K78" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M78" s="6" t="s">
         <v>89</v>
@@ -4486,7 +4543,7 @@
         <v>103.774413</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E79" s="2">
         <v>57</v>
@@ -4498,16 +4555,16 @@
         <v>25</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K79" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M79" s="6" t="s">
         <v>85</v>
@@ -4516,7 +4573,7 @@
         <v>111</v>
       </c>
       <c r="P79" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -4530,7 +4587,7 @@
         <v>103.803037</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E80" s="2">
         <v>35</v>
@@ -4542,19 +4599,19 @@
         <v>25</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K80" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M80" s="6" t="s">
         <v>117</v>
@@ -4571,7 +4628,7 @@
         <v>103.87891999999999</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E81" s="2">
         <v>38</v>
@@ -4583,19 +4640,19 @@
         <v>25</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K81" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M81" s="6" t="s">
         <v>54</v>
@@ -4604,7 +4661,7 @@
         <v>111</v>
       </c>
       <c r="P81" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
@@ -4618,7 +4675,7 @@
         <v>103.82365299999999</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E82" s="2">
         <v>50</v>
@@ -4630,16 +4687,16 @@
         <v>25</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K82" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M82" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O82" s="2" t="s">
         <v>111</v>
@@ -4656,7 +4713,7 @@
         <v>103.72327</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E83" s="2">
         <v>57</v>
@@ -4668,16 +4725,16 @@
         <v>25</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K83" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L83" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M83" s="6" t="s">
         <v>85</v>
@@ -4694,7 +4751,7 @@
         <v>103.90475499999999</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E84" s="2">
         <v>54</v>
@@ -4706,19 +4763,22 @@
         <v>25</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K84" s="2" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M84" s="6" t="s">
         <v>49</v>
+      </c>
+      <c r="N84" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="O84" s="2" t="s">
         <v>107</v>
@@ -4735,7 +4795,7 @@
         <v>103.881266</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E85" s="2">
         <v>35</v>
@@ -4747,22 +4807,25 @@
         <v>25</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I85" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K85" s="2" t="s">
-        <v>163</v>
+        <v>90</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M85" s="6" t="s">
         <v>54</v>
+      </c>
+      <c r="N85" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="O85" s="2" t="s">
         <v>111</v>
@@ -4773,13 +4836,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="2">
-        <v>1.322109</v>
+        <v>1.438226</v>
       </c>
       <c r="C86" s="2">
-        <v>103.847272</v>
+        <v>103.803116</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E86" s="2">
         <v>36</v>
@@ -4790,14 +4853,172 @@
       <c r="G86" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="H86" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>240</v>
+      </c>
       <c r="K86" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L86" s="2" t="s">
         <v>97</v>
       </c>
+      <c r="M86" s="6" t="s">
+        <v>132</v>
+      </c>
       <c r="P86" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>86</v>
+      </c>
+      <c r="B87" s="2">
+        <v>1.353766</v>
+      </c>
+      <c r="C87" s="2">
+        <v>103.75482700000001</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E87" s="2">
+        <v>24</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="J87" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="L87" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M87" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="P87" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>87</v>
+      </c>
+      <c r="B88" s="2">
+        <v>1.322139</v>
+      </c>
+      <c r="C88" s="2">
+        <v>103.84719699999999</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E88" s="2">
+        <v>32</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="L88" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M88" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>88</v>
+      </c>
+      <c r="B89" s="2">
+        <v>1.377157</v>
+      </c>
+      <c r="C89" s="2">
+        <v>103.88187000000001</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E89" s="2">
+        <v>30</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="M89" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>89</v>
+      </c>
+      <c r="B90" s="2">
+        <v>1.322139</v>
+      </c>
+      <c r="C90" s="2">
+        <v>103.84719699999999</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E90" s="2">
+        <v>41</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>